<commit_message>
Get daily reddit data: Tue Mar  4 08:10:33 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_03_09.xlsx
+++ b/data/collected_data/2025_03_09.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C488"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3185 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1j35zax</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Painted my nails for the first time as a man</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j35zax</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1j35kej</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>I’m obsessed! Can you guess why?</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j35kej</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1j35k81</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>I’m obsessed! Can you guess why?</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j35k81</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1j34jzv</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Lifted nail</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j34jzv/lifted_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1j34o5s</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Under-nail skin peeling after shellac</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j34o5s/undernail_skin_peeling_after_shellac/</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1j34kts</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>I hate the bubble gum pink base for acrylics.</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vftnx7dp9mme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1j344pn</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>My work as a nail tech of 4 years✨</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j344pn</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1j33zqz</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>love it 🫶🏼</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j33zqz</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1j33xj9</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Love my nails</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j33xj9</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1j31ywb</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Nail splitting weird always</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/crcxqv38ilme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1j30427</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Are cat eye shades generally translucent on natural nails?</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j30427/are_cat_eye_shades_generally_translucent_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1j2zyz3</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Nail tech help.....❓❓</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j2zyz3/nail_tech_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1j336p6</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Birthday Nails</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j336p6</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1j32v85</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Any tips on rhinestone application?</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j32v85</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1j32nvy</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Nail techs who work In a salon/spa, what nippers are best in your opinion?</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j32nvy/nail_techs_who_work_in_a_salonspa_what_nippers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1j32aww</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Second attempt at DIY</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o7l1qxrcllme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1j31ozr</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Long-nail buddies: how do you floss?</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j31ozr/longnail_buddies_how_do_you_floss/</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1j2zpop</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>What nail shape should I go for? Inspo from u/dk17us on Reddit and Kayla on Tiktok!</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2zpop</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1j318s3</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>I broke my nail bad at work, how can I help the healing process since it's below the quick?</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m2zcm0zdblme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1j31gn8</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>What would you do to improve the Polygel apex?</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j31gn8</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1j30gzc</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>a year of doing my own nails</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vzn4c2s44lme1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1j30caz</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Someone’s favorite color 🫐</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/afd1p11y2lme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1j304at</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Shine nails without nail polish</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j304at/shine_nails_without_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1j307gx</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>How to put on a necklace with long nails?</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u8y5unzn1lme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1j303rf</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>beach nails</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ohnx17xp0lme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1j2zy17</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Matte gold flake 8</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2zy17</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1j2zy04</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Matchy Matchy</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/78f6pno8zkme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1j2wrtg</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>must buys for a beginner?</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j2wrtg/must_buys_for_a_beginner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1j2z1q2</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Gel X for nail tips?</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j2z1q2/gel_x_for_nail_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1j2z0x5</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Advice?</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3vd5yajsqkme1</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1j2yxhp</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>advice plss :(</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2yxhp</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1j2yun6</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>I’ve been trying out different press ons and these have been some of my favorites</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2yun6</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1j2yqzp</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Just finished these pink pearly nails~</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fhuw5mfaokme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1j2yn5y</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>full glam rhinestones + requested Nosferatu hand shadow</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2yn5y</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1j2ylrc</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Advice Needed</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j2ylrc/advice_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1j2y6ar</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Second time ever doing my own nails ☺️</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uacgui1ajkme1</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1j2y4hw</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>are they giving gender reveal? that’s not what I was going for 😭</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gvyu2umuikme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1j2y490</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Green nails after doing my own press ons</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fzbrc1dsikme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1j2y1jp</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>So i dropped something on my nail and this happened, will it be okay?</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/92yziia5ikme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1j2xtf6</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>New Art Deco set</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2xtf6</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1j2xk7f</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Kingdom Hearts Box Art Riku as Nail Art!</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2xk7f</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1j2xg9r</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>What's up with this line?</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xkywod87dkme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1j2xecq</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>7 months of my nails</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2xecq</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1j2xcxm</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>I went and tried out a new nail salon today</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f2oetfbhckme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1j2xa3u</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Purple chrome 😍</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zpjrbglnbkme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1j2x8b0</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Just nails</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/puwcjjncbkme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1j2x1un</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Where do I find extra fine piping tips ?</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1b5ga8ut9kme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1j2x1ep</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Magenta Pink 🩷</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pw1pehnl9kme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1j2wpyj</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Bestie</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nvkxhcm27kme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1j2wh0g</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>can I fix this?? and if I can, how??? (the nail not having skin around it anymore)</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kb6bponx4kme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1j2vzgw</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>To put on false nails or not?</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2vzgw</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1j2vecf</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Help!</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j2vecf/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1j2vnex</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>How do you keep your cuticles nice?</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2vnex</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1j2vv4n</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Shameless copying and thanks for the inspiration!</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2vv4n</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1j2vpp4</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>looks like i should try a different nail shape...</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2vpp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1j2veyg</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Did these last night. Done with my non dominant hand too</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jxsdftxowjme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1j2v9o7</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Ready for spring!</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xeam2w1kvjme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1j2usq2</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Nail glue issues, hoping for some advice</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2usq2</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1j2uiia</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Am I crazy or are my nails not that great…? (TL;DR: not happy with my nails and concern about gel allergies)</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2uiia</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1j2u8fl</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>First DIY Gel Mani</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2u8fl</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1j2ug73</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>My crappy sunflower in support of Ukraine</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jh4iwbuapjme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1j2u8q7</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Do they look professionally done?</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/51e607eqnjme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1j2u5la</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Do I do them or not? 🧐</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ewt5a63njme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1j2u1nd</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Clean girl aesthetic, but for an elder emo: Part 3</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2u1nd</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1j2trwb</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>fresh set 💅🏾</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2trwb</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1j2t91z</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Tip extensions for DIY press ons for flat-ish nail beds?</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j2t91z/tip_extensions_for_diy_press_ons_for_flatish_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1j2s84d</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Swamp Witch Inspired Nails</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/41r4qvzq8jme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1j2tgmz</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Do my nails look ok?</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fzqgt9wzhjme1</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1j2tda8</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Didn’t realize my nails matched my jacket until I showed my fiancé.</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n34k71hahjme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1j2ta9w</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Cobalt+Maldives chrome😍</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z8zafw4kgjme1</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1j2sql6</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Single nail clubbing!!</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2sql6</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1j2stwj</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Square shaping tips?</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9cjcrfh9djme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1j2skxv</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Are these messed up?</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2skxv</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1j2seqq</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>learning piano or having long nails</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j2seqq/learning_piano_or_having_long_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1j2j62j</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Pain on tips?</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2j62j</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1j2jepv</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Bright PINK for the frigid weather!!!</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xn6mwr0yehme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1j2rc97</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Practicing on family and close friends!</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2rc97</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1j2g845</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>How do I remove gel nail at home ?</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j2g845/how_do_i_remove_gel_nail_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1j2k5x8</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>nails after gel</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qh6q7xjelhme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1j2kgz1</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Is it normal to have multiple acrylic nails lift/fall off within two weeks? 🥲</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j2kgz1/is_it_normal_to_have_multiple_acrylic_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1j2mp6e</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Glaize fails</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j2mp6e/glaize_fails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1j2rvcd</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>I recently started getting nail art and omg it’s so fun. I feel like a fairy princess with these nails 👑</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2rvcd</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1j2rwa7</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Butterfly vibes 🦋</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2rwa7</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1j2rum5</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Would you be happy if you got these at a salon?</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2rum5</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1j2role</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>New Set, Light Pink &amp; Rose Gold ✨</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2role</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1j2rjxc</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>essie ink jelly</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j2rjxc/essie_ink_jelly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1j2qylb</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>boyfriend picked the colour and shape</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xtuaq4uczime1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1j2qmzk</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Marilyn Monroe Graffiti Nails 💅</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tp3cxwr6xime1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1j2qar7</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>I too cannot stop doing cat eyes 😻😻😻😻😻</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2qar7</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1j2pz9w</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Green for March, so original!</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2pz9w</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1j2proh</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Did my nails myself for the first time EVER!</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ugxs870rime1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1j2osyd</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>gel manicure after soaking off acrylics… botched?</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2osyd</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1j2onk0</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>New set!</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2onk0</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1j2ocph</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Lil love to my nail girl!</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2ocph</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1j2ntu7</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Natural nails: will acrylic do better than hard gel?</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j2ntu7/natural_nails_will_acrylic_do_better_than_hard_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1j2nqzo</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>💗🍥💫 Pink Set with iridescent chrome</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2nqzo</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1j2nfen</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>The glow this polish gives is insane</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2nfen</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1j2mqkr</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Nail student test</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u7iz8pi25ime1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1j2mpsl</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>First time getting my nails done. It's been two weeks</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2mpsl</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1j2m5an</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Showing off my cotton candy nails that I did myself 🥰 I’m a beginner so this is huge progress for me</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2m5an</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1j35lmg</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Essie To The Rescue Review</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j35lmg</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1j34i72</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>El diseño lo eligió el novio , que les parece??</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ktjcmz7n8mme1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1j3425p</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>The purple polish of my dreams</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3425p</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1j33rnu</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>When your nails match your drink!</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j33rnu</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1j339mi</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Que opinan de este hermoso diseño</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mntxzfululme1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1j336nf</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>My personal disco ball 🪩</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j336nf</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1j32yhs</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>whimsigoth duochrome to bring on early spring vibes 🌱</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j32yhs</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1j32vhm</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | PPU - It’s Tricky</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j32vhm</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1j31sjv</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Que les parece, estos diseños</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j31sjv</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1j31oqk</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>reduced or lanolin free cuticle removers</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j31oqk/reduced_or_lanolin_free_cuticle_removers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1j30vvv</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>I need help finding a good pink polish😭</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j30vvv</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1j30kn3</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>ISO Valentine's Day nail polish (FORGOT THE BRAND)</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j30kn3/iso_valentines_day_nail_polish_forgot_the_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1j2zpjs</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Baby’s first Clionadh 🥲</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/og1olv43xkme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1j2zewk</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>February Nails 💌</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2zewk</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1j2z6cf</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Which polish lived up to the hype for you, and which one did not?</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j2z6cf/which_polish_lived_up_to_the_hype_for_you_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1j2yz38</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Laissez les Bons Temps Rouler</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2yz38</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1j2ym9x</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>opinions please!</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dwpbfne6nkme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1j2xwdu</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Velourilnp</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2xwdu</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1j2xp47</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>where have you psilocy-been all my life?</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jkno9gr9fkme1</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1j2xirp</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Really surprised by this polish! It was under $5! This is Glamengo by LA Colours Neon Jelly’s</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/siwxvn5sdkme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1j2wsyt</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Laissez les bons temps rouler</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2wrnb</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1j2whf9</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>My Set For The Week</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2whf9</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1j2w52h</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Clionadh Norpsilocin, Psilocybin, and Baeocystin back in stock</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j2w52h/clionadh_norpsilocin_psilocybin_and_baeocystin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1j2w2oo</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>The Bubbles</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2w2oo</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1j2vnuo</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Loving this combo!</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/68d8ybeiyjme1</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1j2ui6x</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Holo Taco Customer Service Shout Out</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j2ui6x/holo_taco_customer_service_shout_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1j2u091</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>palate cleanse: some coffee with my coffee</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ut2s5y3wljme1</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1j2tzzu</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Oscars night skittle! One color for each Best Picture nominee</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cot0c56xljme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1j2t2jn</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Where to order from</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j2t2jn/where_to_order_from/</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1j2t0c1</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Holo taco peach tea</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2t0c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1j2slgh</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Shared before then I saw this!</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8svnmmcibjme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1j2scd9</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Lurid - Purple-Eyed Shadow Daddy (HHC Jan ‘25)</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wijzvmxl9jme1</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1j2r95b</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>maelstrom over black 🫡</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ez2w6vxl1jme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1j2r3t7</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Stained glass inspired</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2r3t7</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1j2r17p</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Getting started with velvet nails</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j2r17p/getting_started_with_velvet_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1j2r05s</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Sooo excited about my nail mail</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2r05s</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1j2qq21</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Banquet of Breadcrumbs 🍃</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2qq21</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1j2q9yh</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Mardi Gras Mani 🥳</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2q9yh</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1j2pknx</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>The gender binary is a lie</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/gender-binary-is-lie-0fcNI0y</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1j2paie</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Press-ons I made this week</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2paie</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1j2oyn9</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>How much cuticle oil do you go through?</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j2oyn9/how_much_cuticle_oil_do_you_go_through/</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1j2oh9g</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Red Eyed Lacquer - I’m sorry…Dragons? Those are a thing?</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8ta0j9qrhime1</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1j2o9qv</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Such bright sparkles! ✨</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aa23ztt7gime1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1j2nhuu</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>The light was just right</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ob2zakoaime1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1j2nhuo</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Kismet ✨</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ltjecvcoaime1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1j2naou</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Monster Vibes 🍑</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j1v9a0</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1j2n8ho</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>How do I keep my nails from ripping halfway down the nail plate?</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m4gm120t8ime1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1j2n7nr</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Velour really is That Girl</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4ou5ieni8ime1</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1j2n2ic</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>What happened to my magnet??</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8b9zrx2k7ime1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1j2mlh9</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Ilnp haul!</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2mlh9</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1j2mktc</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Trans Solidarity Collab</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2mktc</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1j2m89g</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>🏳️‍⚧️Trans Solidarity🏳️‍⚧️</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2m89g</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1j2lakg</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Fire Nails</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2lakg</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1j2l43w</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>I adore the colours of the new Ulta lip balms, got inspired to paint these!</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/huah5w5wshme1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1j2klyg</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Glitter grabber in Canada?</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j2klyg/glitter_grabber_in_canada/</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1j2keod</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>La Petite Mort</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2keod</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1j2jtxo</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>i feel like i have opals glowing on my fingertips</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2jtxo</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1j2jni7</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Surprised how much I like this polish 💙</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2jni7</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1j2hys4</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Sparkle Stars</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5np77yvl1hme1</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1j2gp4f</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Mad that i cant capture this polishes true beauty 😭</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2gp4f</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1j2g7hf</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j2g7hf/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1j25f9t</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>PVB still in Fillin' Groovy?</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/201n78l78dme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1j2f29t</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>ILNP Set Sail</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2f29t</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1j2ewfd</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Please help me ID or dupe this purple-y shade with orange yellow shimmer.</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w4zw6dq91gme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1j30nzq</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>I painted my nails to match my branded belt bag I’ll be wearing all week for a trade show 💅🏼💜</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j30nzq</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1j2zx13</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Matchy Matchy</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8yqh8lpzykme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1j2xl53</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Kingdom Hearts Box Art Riku as Nail Art!</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2xl53</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1j2wz20</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Did decoden nails for the first time ^.^</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/logyope69kme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1j2wvve</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>must buys for a beginner?</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1j2wvve/must_buys_for_a_beginner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1j2wvno</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>I was a bit late to jumping on the Pigment Powder bandwagon - but now I don’t think I’m ever jumping off it 😆🎨</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2wvno</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1j2wosm</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>I think I found my new tech! (bylilithrose)</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/atzks8nt6kme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1j2w5jm</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Vampire nails ♥️🖤🥀🧛🏼‍♀️</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2w5jm</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1j2vygk</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Nails for my boyfriend 🥰</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ufkpb3x0kme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1j2vsi2</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>today's nails</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yfv9983mzjme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1j2vhon</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>👺🎏🍥Demon Slayer Nails I made for a friend! What do you think? Hashiras vs Demons</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2vhon</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1j2sxm5</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Do you love a plaid mani? ☘💛💚🖤🍀</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2sxm5</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1j2sn2p</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>MPA Advanced Painting Gel Neon Color Palette Review</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2sn2p</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1j2r6k7</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>The joy I felt when I realized I could make nails to match my jacket 😍</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wt5zs9o11jme1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1j2qpud</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Started doing my own nails, here’s a couple of my first few practice attempts at some fun designs!</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2qpud</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1j2qo4m</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Are there any dos and don’ts of using 3D gel?</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1j2qo4m/are_there_any_dos_and_donts_of_using_3d_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1j2qntm</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Marilyn Monroe Graffiti Nails 💅</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/auxuv2pcxime1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1j2pwxb</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Forest fairy 🧚🏻</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2pwxb</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1j2o3ja</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>🪩✨🐈‍⬛ Cat eye x Chrome I did</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wa64r3eyeime1</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1j2lopr</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>These keep distracting me from reading 😍✨</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qqtxwx9axhme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1j2llrm</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>First time trying design on my nails</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cm1spc2nwhme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1j2lcu0</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Fire Nails</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2lcu0</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1j2iwn5</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>My friends pick up this set, they wanted a fairy etherial stilleto with purple accents did I deliver?</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j2iwn5</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Mar  5 08:11:24 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_03_09.xlsx
+++ b/data/collected_data/2025_03_09.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C488"/>
+  <dimension ref="A1:C675"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8729,6 +8729,3185 @@
         </is>
       </c>
     </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1j3y5og</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>I don’t like traditional french white tips and asked for something a little different</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t1s58e7ivtme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1j3x67j</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Uneven Nail Beds</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0wa7esojitme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1j3x7i8</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>I don’t have a nail but that doesn’t stop me</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pwwmxkyzitme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1j3x2oe</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>First time using gel polish</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3x2oe</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1j3wu3u</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Okay so what are these lines on my nails whats wrong?</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xjv7xligetme1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1j3v9y4</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>How can I recreate these nails? From bghofrane966 on Pinterest!</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vtpj9g9hxsme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1j3w9bf</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>tiny nails</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3w9bf</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1j3vqb5</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Narrow nails and long fingers - best shape for them?</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y4ecam712tme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1j3vdy5</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Really diggin’ my birthday set!</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3vdy5</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1j3v03t</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>First attempt at sns with tips</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3v03t</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1j3upib</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Black French and bows</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3upib</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1j3udcf</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>i’ve tried everything - help!</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a0i49w6cosme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1j3u4m4</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Does anyone else’s nails look like this?</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f0wd9lgvlsme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1j3tkh7</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Nail gap?</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j3tkh7/nail_gap/</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1j3t4mu</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Tips for getting gel nails to stick better?</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j3t4mu/tips_for_getting_gel_nails_to_stick_better/</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1j3ukcp</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Shell Nail 🐚</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3ukcp</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1j3ubxo</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>my new nails 🤍</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oxot6ejxnsme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1j3u9eo</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>My Nephew Had A Birthday Party Last Weekend And I Got my Nails Done Last Monday To Fit The Nike Theme 👟</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nx7yz9e7nsme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1j3u7w2</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>First time doing my own gel w/ acrylic extensions ☺️</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3u7w2</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1j3u2kz</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>best nail glue for press ons???</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j3u2kz/best_nail_glue_for_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1j3tkuo</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>I got my nails done on Valentine’s Day</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uzuzem9lgsme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1j3te20</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>First time with a shape other than square</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3te20</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1j3tc76</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Anyone know of a colour named “I don’t care”?</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j3tc76/anyone_know_of_a_colour_named_i_dont_care/</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1j3tbq0</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Wide nail beds</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c8jzrasaesme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1j3s95n</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>trying something new</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3s95n</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1j3rt6e</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>In love w my new set!</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3rt6e</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1j3rqfe</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>These feel so sunny and warm</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3rqfe</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1j3r67g</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>What shape nail would look beat with my fingers?</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ldh1g4f1vrme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1j3qlq6</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Gel nail and doing your dominant hand tips/tricks</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3qlq6</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1j3p62k</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Training to be a nail tech and spent way too long on these 😂</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t8702n97erme1</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1j3qcn1</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Glamnetic press on remover question</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j3qcn1/glamnetic_press_on_remover_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1j3q75e</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Trying fake nails for the second time</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9jmxkcdqmrme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1j3q1tj</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Wishing for Spring/Summer</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3q1tj</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1j3pyck</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>acrylics damaging my nails, looking for alternatives</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2456eamnkrme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1j3pp5x</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Gel x</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j3pp5x/gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1j3poty</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>What shape suits me best?</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3poty</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1j3oilm</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>How to get a sharper look around nail bed</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ochr8ur09rme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1j3ouci</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Loved the tiles in this shower</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j3ouci/loved_the_tiles_in_this_shower/</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1j3otdi</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Do you like them? They are simple but pretty</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mhu2pgkebrme1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1j3okoj</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>I love my nails with the cat eye effect, do you like them?</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dr3yzsyg9rme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1j3oh7x</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Purple-Eyed Shadow Daddy is breathtaking</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3oh7x</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1j3mmbd</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Is this normal damage from gel removal?</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pfqyn9tjuqme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1j3mgwm</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Hypoallergenic press on nail glue alternatives?</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j3mgwm/hypoallergenic_press_on_nail_glue_alternatives/</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1j3kq7v</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Matte with shiny tips</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r7txt8pfgqme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1j3nnfs</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Finding a new nail tech has been HELL</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j3nnfs/finding_a_new_nail_tech_has_been_hell/</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1j3ob4z</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Do you do duck nails? Me:</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1z8cqnzc7rme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1j3nyh4</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>My nail artist is so incredibly talented; this counting sheep set is too cute!!</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j4dm351n4rme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1j3nx3j</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>What makes you like square nails/dislike almond nails?</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3nx3j</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1j3ncm1</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Accent/party nail</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3ncm1</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1j3n4s5</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>My biab nails</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3n4s5</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1j3n2p8</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>I told her to do whatever she wanted</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3n2p8</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1j3mzn9</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>The new new</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3mzn9</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1j3mz61</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>[Repost.] St. Patrick’s Day</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/w1kea067xqme1</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1j3mgvw</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Holographic</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m3zaah2gtqme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1j3mcbd</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Are my nail beds too wide for this shape?</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3gjxnc7hsqme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1j3mbe0</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>My first time having square in 10 years</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f6vwbrmcsqme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1j3m74g</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Leopard Nail Gang</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3m74g</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1j3lzzi</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Lo lindo de ser manicura, es que haces arte</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3lzzi</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1j3lu3s</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Que les parece, están delicadas ??</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/24q0hw2noqme1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1j3lirk</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Nail shape help.</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3lirk</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1j3las8</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>first ombré almond nails</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3las8</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1j3kwje</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Is it worth it getting your own setup?</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j3kwje/is_it_worth_it_getting_your_own_setup/</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1j3ktxn</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>White polish that doesn’t streak?</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j3ktxn/white_polish_that_doesnt_streak/</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1j3kgk9</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>I'm in love with my cat nails!</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hnipiv5geqme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1j3k2y4</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Proud of myself</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8m7mc7unbqme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1j3k1pw</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Barbie Earring Magic - Ken</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3k1pw</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1j3j3ji</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Pricing?</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3j3ji</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1j3jgu3</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Need nail tips for wedding and inspo for a natural look</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j3jgu3/need_nail_tips_for_wedding_and_inspo_for_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1j3jzd8</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>i bought flawless nail salon drill pretty powerful motor</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wigdfunwaqme1</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1j3jzeh</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Art House by DND 🥰</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g9vfo3ozaqme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1j3jvm8</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Strawberry frenchies</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rz6rtoy7aqme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1j3jpld</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>New set 💅🏼 feeling galactic 🌌</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3jpld</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1j3jfsl</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>I was a rock climber for a very long time so I couldn’t have pretty nails</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/onhflpxy6qme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1j3je1k</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Canadian Acrylic Brands?</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j3je1k/canadian_acrylic_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1j3jano</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Goggly eyes on nails</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a7t7yvgx5qme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1j3ja06</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Sculpted these hush puppies</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jqek8pus5qme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1j3j29n</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Are the nails too wide or is it just my natural nail ?</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/907xwap84qme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1j3is4f</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>I absolutely loved these in the packaging</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3is4f</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1j3igk2</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Tried coffin for the first time ever and I think I’ve found my favourite nail shape!</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hjajm48wzpme1</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1j3ia27</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Ready for spring!</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mtnclu2mypme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1j3i1iv</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Spring ready 🌼</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/49z481iuwpme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1j3fclh</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>first time getting my nails done can u guys help</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3fclh</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1j3bya3</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>rouge the bat- sonic inspired nails 🦔</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/snq6957gnome1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1j3dlms</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>How do you get ink out from under acrylics!?</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lgvlhu6r0pme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1j3f38h</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>newest set : grimace nails 💜</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m7l963xsbpme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1j3fegx</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>first time getting my nails done can u guys help</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3fegx</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1j3felb</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Aggressive Manicuring: Permanent damage?</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3felb</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1j3fffa</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Second set of nails ever!</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3fffa</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1j3fmv4</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Tips for gel polish newbie!</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j3fmv4/tips_for_gel_polish_newbie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1j3gp3c</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>A little bit of my nail journey</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3gp3c</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1j3hqyl</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Tips and tricks to grow out nails for nurses or nursing students?</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gy8vkqwqupme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1j3hjkd</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>What kind of manicure did I get?</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mfa2v5oatpme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1j3hdu1</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Does anyone else prefer solid colored simple nails?</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j3hdu1/does_anyone_else_prefer_solid_colored_simple_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1j3g9xu</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Spring flowery nails 😊🌼🌸</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3g9xu</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1j3fshu</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>I absolutely hated my nail shape so I cut them myself</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3fshu</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1j3exy6</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>First time doing french tips myself... How did I do?</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rtxqxn8papme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1j3edxm</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Loving my Green Velvety Nails!</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3edxm</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1j3edhd</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Guys how to trim your nails the correct way? Mine always look like I've returned from a war</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j3edhd/guys_how_to_trim_your_nails_the_correct_way_mine/</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1j3e0dl</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Favorite Etsy shop for press ons</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j3e0dl/favorite_etsy_shop_for_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1j3dzmr</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>I wanted to try black nails for a loong time🖤</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3dzmr</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1j3wh3j</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Shoulda known this would happen…</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7eo6q8v3atme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1j3vypi</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Looking for nail basics recommendations (primer, top coat, thinner?)</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j3vypi/looking_for_nail_basics_recommendations_primer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1j3vxs8</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Forbidden Fruit</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vip6kitc4tme1</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1j3vfpi</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Really proud of my mani this week</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3vfpi</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1j3v747</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Mardi Gras Masquerade</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dv0j6a4nwsme1</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1j3uyy9</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>I've fallen into the rabbit hole of making my own nail polishes</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3uyy9</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1j3t9ec</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>On today's episode of "I can't believe this is all the same polish"</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/holpbyfqdsme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1j3snn3</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>What are your favorite magnetic polishes for the velvet effect?</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j3snn3/what_are_your_favorite_magnetic_polishes_for_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1j3sged</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>First time I've swatched an order immediately after it arrived.</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ma0kf8xf6sme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1j3s5dz</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>SO GLOWY!! Ghosts of Hecate</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3s5dz</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1j3rzbb</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Springy Nails</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3rzbb</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1j3rl0i</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>my new go to red 🍎🐈‍⬛</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3rl0i</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1j3qd8k</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Need help finding IDing LA Girl shade</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3qd8k</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1j3phvb</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>I know we criticize indie brands with bad swatch photos, but can we just take a moment to acknowledge how much better they are than OPI, etc?</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3phvb</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1j3pese</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Never Let Me Go from Prism Polish’s Valentine’s collection</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3pese</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1j3peni</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>No polish bare days. Always wanted to post this.</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/980c3t07grme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1j3p1hy</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>I can't believe she's going away</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3p1hy</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1j3oo2j</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Magnetic skittle</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dtmedr27arme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1j3non5</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>I’m Blue 💙</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3non5</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1j3nk5f</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Would you contact customer service about the lack of visible glitter in Supernova (the purple one)?</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3nk5f</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1j3nht9</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>My assortment of nude polish for new regulations</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3nht9</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1j3n9nc</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>What I wore in February</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3n9nc</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1j3n7vg</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>post update!</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3n7vg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1j3n5q3</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>POV doing the dishes and going to the toilet</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3n5q3</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1j3mxg0</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Sunset-looking polish recs</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j3mxg0/sunsetlooking_polish_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1j3msra</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Glitter grabber question</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j3msra/glitter_grabber_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1j3mazp</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Am I addicted to multichromes now?</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nh92uzh9sqme1</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1j3m9m6</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Sending out a subreddit-wide beacon for fellow Star Wars fans! 🌌🪐</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3m9m6</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1j3m5ng</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Pop Art inspired French Tips</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8tfta1dxqqme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1j3l7xk</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>At least 2 weeks with O, Dauntless, Guarded Beauty (Lurid Lacquer). Absolutely love it. It’s the kind of nail polish that hypnotizes you with the glitter and color shifts</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3l7xk</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1j3l6vn</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Taking nail polish from US to UK</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j3l6vn/taking_nail_polish_from_us_to_uk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1j3l3sa</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Clionadh is my new obsession</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3l3sa</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1j3l0pq</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Honeymoon + Key Drama</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3l0pq</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1j3ky9r</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Clionadh Recommendations</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j3ky9r/clionadh_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1j3knih</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Tried Water Marbling for the First Time in Years</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bn6p5uzgfqme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1j3k5sw</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Discovered a Good Combo</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l8b1r37vbqme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1j3k4gi</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>It can be done! Using up three colour polishes.</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eovm4wyybqme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1j3j7zh</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>I'm obsessed with my cat nails</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qvjqz2ue5qme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1j3j7wx</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>should I avoid gel nail polish if I have a long history of contact dermatitis/eczema?</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j3j7wx/should_i_avoid_gel_nail_polish_if_i_have_a_long/</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1j3j2gm</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>China Glaze pick up</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n92wzm7a4qme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1j3i6c9</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Everything, Everywhere, All at Once</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dlmqofuuxpme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1j3i4k8</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>First attempt at free hand French gel nails</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3y6h0gxhxpme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1j3h5bi</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Blowin Bubbles boosts morale!</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3h5bi</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1j3h0lf</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Essie - Off Tropic</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3h0lf</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1j3gyky</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>I want to love this SO bad</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ny5lq446ppme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1j3gyix</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>i lost the fight with a doorframe</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3gyix</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1j3gtoc</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>I did a thing</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3gtoc</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1j3gaid</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Tried Seche Blur - Before/After</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3gaid</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1j3g9zp</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>February Nails</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5xpd20q9kpme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1j3fuls</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Happy Fat Tuesday! ft. Mardi Gras Masquerade by Kathleen &amp; Co</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3fuls</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1j3frax</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>It Was Worth It 🍎🥧</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3frax</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1j3fbjc</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>I know it's a base coat, but I'm kinda feeling it</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jnx7to5gdpme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1j3f05w</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Grass green sea glass</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3f05w</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1j3eq0s</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>L.A Color Asteroid 😍</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3eq0s</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1j3dvy6</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>My journey through chrome powder on regular lacquer</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pjqxaoyy2pme1</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1j3dpz9</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Learning to love sheers 🌷💗</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6rdbo1mh1pme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1j3dphs</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>drugstore regular top coat recs?</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j3dphs/drugstore_regular_top_coat_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1j3dojg</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Trans Solidarity 🏳️‍⚧️ You exist! You matter!</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2p1gjw1e1pme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1j3de40</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Didn't immediately love this one but it's growing on my ✨🦄</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3de40</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1j3d704</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Petals💖</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3d704</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1j3d41x</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Glowing shimmer - love this for the price!</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3d41x</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1j3caik</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Polish recommendations with a mix of these colors?</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a8h71u1cqome1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1j3b1t9</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>🩵💙RGB Split Illusion❤️💛</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3b1t9</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1j3azon</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Clearance Haul!</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3azon</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1j38s4y</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Dupes for Essie Ballet slippers?</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j38s4y/dupes_for_essie_ballet_slippers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1j382se</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Very proud of how these little magnetic flowers came out</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j382se</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1j37xc1</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>How to heal cuticles?</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j37xc1/how_to_heal_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1j365av</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>February Nail review!</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j365av</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1j2w67h</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Melodysusie UV Lamps good?</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j2w67h/melodysusie_uv_lamps_good/</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1j3wbqa</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Strawberry shortcake nails!</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3wbqa</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1j3u6yl</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Pisces In progress</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/82sc0dzimsme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1j3tx3z</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Gojo nails by me</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t2rgkoerjsme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1j3to1y</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>My nails 💕</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3to1y</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1j3tmca</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Nail Award App</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1j3tmca/nail_award_app/</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1j3swvp</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Shell Molds!! 🐚</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3swvp</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1j3stb8</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Rhinestone Glue for 3D texture?</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1j3stb8/rhinestone_glue_for_3d_texture/</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1j3o0ou</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>The cutest little counting sheep nails done by my incredible artist!</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3wrwsmv35rme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1j3k39g</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Barbie Earring Magic - Ken</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3k39g</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1j3izyq</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Frankie Stein from Monster High inspired nails</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3izyq</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1j3i4pj</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Matte or glossy top coat?</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wr1twr6jxpme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1j3hvq9</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Getting ready for spring 🌼</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1mjtviupvpme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1j3hc79</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Going to a witchcraft museum exposition, I made these nails to wear on that day what do we think?</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3hc79</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1j3f6dx</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Which breed should I try next?🤔</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j3f6dx</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1j3de9i</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Hiii! What nail shape, length, and color/art would make me look like a girly girl?</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1j3de9i/hiii_what_nail_shape_length_and_colorart_would/</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1j3bv82</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Crisp and thin lines???</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aqa7abxomome1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1j37dpz</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Im a new nail tech 🩷 how did I do?</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nqlurb28bnme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1j3769h</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>TIL I love the way stars look but hate drawing them.</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n1q2776f8nme1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Mar  6 08:11:23 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_03_09.xlsx
+++ b/data/collected_data/2025_03_09.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C675"/>
+  <dimension ref="A1:C866"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11908,6 +11908,3253 @@
         </is>
       </c>
     </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1j4puid</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Right on time for island getaway 🏖️🐚🌊</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4puid</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1j4pnau</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Theme was Galaxy / Space, did i nail it?</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1ujp0hn3o0ne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1j4pgdn</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>3D Chrome Snakesssss</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4pgdn</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1j4out7</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Swipe for the *magic*</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4out7</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1j4okc2</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>nail growth before n after</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4okc2</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1j4nugy</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>One of my kuromi decals fell off at work 😿</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kbo9uasl30ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1j4o7qj</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>I'm learning to do my own nail decorations, do they look pretty? And how much do they give them from one to ten?</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4o7qj</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1j4nnwj</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Need advice!</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j4nnwj/need_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1j4nmx5</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>O Canada!</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4nmx5</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1j4m0cj</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Acrylic nail cracked after repair, please help this acrylic nail newbie with advice!</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4m0cj</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1j4mdym</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Question: Manicure inspo credit: @a-chan and @Becky on Pinterest</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4mdym</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1j4mn2u</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Blue ombré</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p2qznmnbrzme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1j4mgcd</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Red french tips</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4mgcd</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1j4maqu</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Black with pink and silver chrome</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/25dbibfynzme1</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1j4m9f4</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Clear coat gel polish.</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nk9nf3vjnzme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1j4m575</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>¿What do you think?</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n4w5vd3hmzme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1j4m0gv</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>I saw this idea on this page, and I think I love this new color. It looks very elegant</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7fr37m48lzme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1j4lyac</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>What do you think of the new color?</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xxoxmd8okzme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1j4lrhv</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Gel at home</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j4lrhv/gel_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1j4l87h</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>First attempt at aquarium nails💕</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t9u9jra3ezme1</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1j4l2kf</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>the nails i got married in</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qa4mafzoczme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1j4kn6f</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Can someone please recommend a color like this??</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rl9r3gzx8zme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1j4kp31</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Today's nails were peacock inspired</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4kp31</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1j4kr1h</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Totally OBSESSED!</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x0rfvfjt9zme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1j4ke20</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Educate me please on builder gel</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5kgu7txp6zme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1j4kh0w</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>March set!!</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4kh0w</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1j4k1s8</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Ombré?</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j4k1s8/ombré/</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1j4jxc4</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Any advice for further improvements to the technique?</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5zoi3rml2zme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1j4jdw2</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Love getting inspo from this sub 💚</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4jdw2</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1j4jh8n</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>My cat eye nails match the scenery</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m2z82yasyyme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1j4jdb9</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Opinions/Reviews of my nail tech</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4jdb9</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1j4j35k</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>I once was poison ivy, but now I'm your daisy</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j6pfcpgdvyme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1j4iswt</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>carnival nails</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4iswt</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1j4iiml</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>This week’s mani</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4iiml</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1j4ihg6</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Did press ons by myself. Did I do these right?</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jz3wan36qyme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1j4i2u6</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>can I use builder gel to extend length?</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j4i2u6/can_i_use_builder_gel_to_extend_length/</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1j4hfp5</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>thoughts?</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4hfp5</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1j4haqm</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Beachy vibes?</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bgrdzdosfyme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1j4h8bo</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Galarian Weezing fluid art</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4h8bo</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1j4fhls</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Sudden press on nail glue allergy?</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j4fhls/sudden_press_on_nail_glue_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1j4h5d6</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Happy (almost) spring! 🌸</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g7a38d2neyme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1j4gs8y</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Soft gel nails says gel glue doesn't need curing.</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iyskop2wbyme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1j4f3as</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Tropical Spring</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4f3as</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1j4gq1c</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>March set</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4gq1c</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1j4gozp</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>I'm in love with these.. Could possibly be a bit more pointy- but I like them.</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rqwmsuv6byme1</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1j4fqup</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Question about my nail bed</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e420as5b4yme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1j4fqd9</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Any good non-UV nail glue on Amazon?</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j4fqd9/any_good_nonuv_nail_glue_on_amazon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1j4f0t2</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>What should I do?!</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j4f0t2/what_should_i_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1j4cx5n</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Products to prevent nail breakage and to help polish stay on better</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j4cx5n/products_to_prevent_nail_breakage_and_to_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1j4e1q5</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>help with my nails!!!</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bjwyng06sxme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1j4ek5u</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>new nails for a concert i’m going to!</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4ek5u</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1j4da6r</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Split nail - Still fill?</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/892hm4upmxme1</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1j4dup6</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>miami x art deco</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4dup6</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1j4egei</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>march nails 🦋🩵✨</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4egei</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1j4eeyq</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Is this shape wrong for me? Would square be more flattering?</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4eeyq</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1j4e7mw</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Square or almond?</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4e7mw</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1j4e5y7</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>I want to eat them 🤤🍬🍭</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y0r4x890txme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1j4dwda</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Anything i can do?</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4dwda</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1j4dt7d</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>My nail tech hit it out of the park</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4dt7d</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1j4btwc</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Tips on cuticle/nail prep for natural nails/regular polish?</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4btwc</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1j4dakv</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>How long did it take you to get used to wearing nails at work?</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4dakv</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1j4dobp</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>The only thing my creativity could come up with this night!</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a1k3hh9jpxme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1j4dhnj</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Best manicure for a brittle nailed bride?</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4dhnj</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1j4bmqz</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Sparky approves of the new set</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4bmqz</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1j4bivc</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>The brief was pink and chaotic and I think my artist nailed it</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4bivc</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1j4b4zs</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>3 months without biting my nails</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4feegy857xme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1j4b1at</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>second time doing my own nails (gel extensions + gel polish)</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zi7w1nnf6xme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1j4axhp</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Gel vs Dip Powder for Shorter Nails</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j4axhp/gel_vs_dip_powder_for_shorter_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1j4as4h</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Chose two colors for my two personalities 😆</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/am53npgq4xme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1j4aqnu</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>first time acrylics!!</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4u79rq9g4xme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1j4alst</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>THE WORST ACRYLICS EVER</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4alst</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1j4adwt</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>matching with my gf</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4adwt</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1j49s61</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>I feel like the colour doesn't match my skin, what do you think?</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0wzbnr9oxwme1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1j49s4y</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>How often do you get your nails refilled before eventually getting a brand new set?</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j49s4y/how_often_do_you_get_your_nails_refilled_before/</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1j49i0t</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Dies this nail shape suit me?</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j49i0t</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1j49fd2</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Why do I hate them?</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jdqg1u35vwme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1j49ev9</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Pretty happy with how this press on nail set came out.</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xcg7ecb1vwme1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1j49dae</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Went for a toasted pink sugar vibe. Is the brown/pink ombré too subtle? I don’t know if I hate this!</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b3z4n5tquwme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1j48cx6</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Side Growth Advice :(</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7v4g0mennwme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1j480fy</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Press-on sizing</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j480fy/presson_sizing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1j47kbj</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Ingredient difference between nail glue and generic super glue?</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j47kbj/ingredient_difference_between_nail_glue_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1j47d9c</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Does this look good, I'm a starter.</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a68mrv0hgwme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1j45ew1</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Nails are more than just an aesthetic</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j45ew1/nails_are_more_than_just_an_aesthetic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1j49aq1</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>the cutest little glitter ombre nails with holographic gold for my mom ❤️🌹🌟</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j49aq1</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1j499p3</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>I’m working on setting up an online store-Thanks to you guys.</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j499p3</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1j48z93</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Should I complain about my nails?</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j48z93</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1j48ggf</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Love black frenchies 🖤</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j48ggf</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1j48f85</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>First time i’ve gotten my nails done in years</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j48f85</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1j48esa</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>🐆🌸</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j48esa</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1j48cm3</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Just made this tie dye beauty</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j48cm3</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1j47e8v</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>previous sets I’ve done on myself</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j47e8v</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1j4747x</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>How can I cover these acrylic gel nails or remove them?</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ng5l595lewme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1j4717r</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>thoughts?</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4717r</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1j46vh6</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Which nail shape suits me best?</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j46vh6</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1j45r8u</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Discolouration?</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/290foebc4wme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1j45vxp</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>The worst acrylics ever</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j45vxp</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1j46tia</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Never had stilettos before but I'm diggin it</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xfayyufgcwme1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1j46r9v</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Valentine’s set</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j46r9v</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1j420zs</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Should I remove my gelX now, even though I'm getting a new set next week?</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dbx9kki58vme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1j41o5l</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Paranoid about applying press ons correctly</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j41o5l</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1j4qmyl</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Finally happy with my light blue glass nails’ effect</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/55ias5dz01ne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1j4qk63</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Show me your jelly sandwiches!</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4qk63</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1j4pu5w</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Thermal w/ light tips?</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l6f164ulq0ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1j4ozub</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Clionadh Cosmetics Tart</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4ozub</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1j4ow2j</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>gold french tips with clear base</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gmxj2qf0f0ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1j4om5z</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>the nailtechs subreddit didn't allow this question, but is it uncouth to ask a nail tech to apply a fake set for you?!</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j4om5z/the_nailtechs_subreddit_didnt_allow_this_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1j4o8pp</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Dollar Tree Nail Art Haul</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j4o8pp/dollar_tree_nail_art_haul/</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1j4nysx</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>February Round Up</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4nysx</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1j4nfw7</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Can anyone guess my favorite color right now…</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4nfw7</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1j4mvb5</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>is it obvious that these are press on nails?</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4mvb5</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1j4mpyu</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Fun</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6gfd1w95szme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1j4mc2e</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Zoya Oceane</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4mc2e</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1j4ktq5</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Clionadh - Doppelgänger</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0laphbbhazme1</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1j4dk8t</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>First ILNP order✨</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4dk8t</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1j4k1vi</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>My favorite “neutral but kinda weird” shade</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4k1vi</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1j4ivc6</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Inadvertently gave myself a very bisexual mani today!</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4ivc6</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1j4h7jc</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Galarian Weezing fluid art</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4h7jc</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1j4h5yr</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Accidental glittery chocolate</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xjsm67sreyme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1j4glxk</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Mani😍</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4glxk</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1j4gas1</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>PfD Lush is phenomenal</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4gas1</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1j4fvaf</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>finally upgraded from 11pro to 16, so i had to paint my nails to match</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4fvaf</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1j4fos6</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Please help me dupe this polish I will die without it.</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4fos6</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1j4fh3v</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Did I finally find my perfect nude?</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4fh3v</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1j4f8ut</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>My neighbor complimented my nails and noted how they matched my pooper scooper 😂</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4f8ut</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1j4exnk</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>I practically ripped the package out of my mailman’s hands</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4exnk</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1j4ett4</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>ILNP Skittle 🧡🩷💜💙</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4ett4</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1j4erdw</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Laissez les bons temps rouler - take 2</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j4erdw/laissez_les_bons_temps_rouler_take_2/</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1j4eh7k</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Love for Mooncat's Millennia (and a cry for help!)</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/61lk1g95vxme1</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1j4du07</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>thermals are so fun for me as a reformed nail biter!!!</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4du07</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1j4d0ii</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Question- Polishes that can’t be used?</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j4d0ii/question_polishes_that_cant_be_used/</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1j4crr5</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Looking for green, blue shimmer topper</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hqjuit00jxme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1j4cnal</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>My nails are helping me through a difficult day of visa rejection</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kw66gue3ixme1</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1j4cmom</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Black Skittle 🖤</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4cmom</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1j4ciel</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>China Glaze Clearance / End of an era?</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p5szjj24hxme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1j4c21d</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>✨️Sparkly Hump Day✨️</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4c21d</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1j4baca</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>First Holo Haul 💿🌮</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/le7ikna98xme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1j4b7ty</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>ILNP Sugar Plum - Obsessed!</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4b7ty</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1j4b5kv</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>So pretty the camera can't focus</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rnz460hb7xme1</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1j4az33</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Why pick one when you can wear them all?</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8i26d7l06xme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1j4ap5k</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>'Tis the sneezon in the Pacific Northwest 🌳🌲🌷🌤</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4ap5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1j49t2s</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>In honor of cleaning the gutters… Tannins in the Leaves</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tlyop6luxwme1</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1j49nfp</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>My Wife Picks Mani: Part 9</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j49nfp</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1j49kwm</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Alone Isn’t So Bad, I Like Alone</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j49kwm</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1j491a8</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>ORLY “Don’t Pop My Balloon” 🩷</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8bksaudgswme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1j48k3b</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Curvature of the nails?</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/adbt0yh1pwme1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1j48ejo</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>What quick dry top coat is the best?</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j48ejo/what_quick_dry_top_coat_is_the_best/</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1j48do7</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Side Wall Growth Advice :(</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ebw1o8osnwme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1j488od</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Cold Heartedness</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j488od</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1j47z94</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Have I ruined my nail polish?</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b1oh0inwkwme1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1j47omt</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Cirque - Cloud Nine</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/njjs6ttuiwme1</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1j47awn</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>These replacement brushes are a game changer!!!</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://a.co/d/aTvuXTj</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1j471ve</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Behold, the finginator! 🧲</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j471ve</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1j46umy</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Is my experience with phoenix’s nail polish normal?</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j46umy/is_my_experience_with_phoenixs_nail_polish_normal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1j46nvs</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Sea glass smooth velvet lacquer</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vs6gmh6bbwme1</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1j467cf</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>How many ILNP collections per year (and when do they drop)</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j467cf/how_many_ilnp_collections_per_year_and_when_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1j45r36</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Dupe request!</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u09jo13b4wme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1j3gky2</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Patty Lopes - Renaissance</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1vd2qp8dmpme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1j3otoa</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Favorite Polishes</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s8yhfuvgbrme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1j3tf61</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Crisp thermals that look like French tips?</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j3tf61/crisp_thermals_that_look_like_french_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1j3ysnx</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Help 🩷</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/was6l4r94ume1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1j43rya</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Do ya’ll think I could *actually* be a swatcher?</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j43rya</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1j43ai8</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Black Maelstrom</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9kc175l2kvme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1j4393p</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>How to get used to longer nails?</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j4393p/how_to_get_used_to_longer_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1j42kim</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Finally figured out my shade of red is scarlet, not cherry</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j42kim</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1j42iik</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Sooooo Shifty! Polar Light Show - What’s Up Nails</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lsg8fiskcvme1</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1j41giq</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>DAM Nail Polish - Quantum Quest</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j41giq</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1j3zyvc</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>I’m feeling a little blue…</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pj1gmbd3kume1</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1j3yfhe</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Cornflower blue for spring</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hlkx6195ztme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1j3yb1x</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Siren 🧜‍♀️</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v8xi6nngxtme1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1j4qj7d</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Flower Nails 💐</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fex2i6fmz0ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1j4pquf</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Theme was Galaxy / Space!</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/c1mwehfdp0ne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1j4mmxi</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Best beginner nail art kits/supplies to buy?</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1j4mmxi/best_beginner_nail_art_kitssupplies_to_buy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1j4mksk</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Blue ombré</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xae9123pqzme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1j4m8jj</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>nail sets I've done recently ! :)</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4m8jj</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1j4m6dm</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>True north strong. 🇨🇦</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5qhnzihsmzme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1j4lb0g</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>i’m very happy with this set.</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4lb0g</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1j4j0i0</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>On myself again 💜</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fip4rabquyme1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1j4hzsm</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Enchanted forest 🌿🍄✨</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4hzsm</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1j4he6q</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Pack a custom press-on order with me 💅🏼</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6p1zgogjgyme1</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1j4fci8</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Any good non-UV nail glue on Amazon?</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1j4fci8/any_good_nonuv_nail_glue_on_amazon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1j4f5hd</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Tropical Spring</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4f5hd</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1j4ejm2</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Latest set on myself</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4ejm2</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1j4c69o</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Getting prepared to open shop!</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4c69o</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1j4b67w</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Need Help</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://pin.it/51krHkGA9</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1j4b63d</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>I made these fairycore-inspired nails, for spring!</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1j4b63d/i_made_these_fairycoreinspired_nails_for_spring/</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1j49k31</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>KB Shimmer Crushing It velvet nails style</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fw8eitrzvwme1</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1j49js0</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>bunnies in the garden 🐇💐</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j49js0</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1j499qr</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>the cutest little glitter ombre nails with holographic gold for my mom ❤️🌹🌟</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j499qr</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1j493l1</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>3D jelly fish nails ⋆˙⟡♡ everything is hand sculpted by me!</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j493l1</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1j461km</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Jelly plaid for spring 💐</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j461km</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1j42nvp</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Do we hate them</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oecxggidevme1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Mar  7 08:11:14 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_03_09.xlsx
+++ b/data/collected_data/2025_03_09.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C866"/>
+  <dimension ref="A1:C1047"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15155,6 +15155,3083 @@
         </is>
       </c>
     </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1j5ije2</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Metal Nails Update</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5ije2</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1j5ht2g</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Obsessed with this micro french manicure 😍</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5ht2g</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1j5hrtv</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>spring nails are here! a design set I did for my client today 🌷</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xa2qz0zyv7ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1j5hcr6</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>; im soooo obsessed with this set😍</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t9o9bploq7ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1j5gm0s</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Can you use a nail hardener on your nails then apply a gel coat to secure a press on /gel x nail?</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j5gm0s/can_you_use_a_nail_hardener_on_your_nails_then/</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1j5gcfe</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Is it giving e-girl?</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wokyj3nye7ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1j5g83p</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>March set!</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fqti8cwkd7ne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1j5flaz</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>How are my nails?</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/20u1kjbv67ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1j5fe8j</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Ladybugs and butterflies and leafy greens</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5fe8j</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1j5ez2z</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>I'm getting my new set tomorrow so here's a goodbye to this magical purple set💜</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q96kkpge07ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1j5eej5</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Can you ever have too much sparkle?</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jc9r1ytqu6ne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1j5eef2</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Cat eye nails!!!</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pfelswgpu6ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1j5e4om</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Bachelorette weekend nails</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nhzfjgy3s6ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1j5dwn8</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>In love with the colors</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.redgifs.com/watch/peachpuffableadouri</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1j5dv56</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Broken nail bed (I think) - next steps?</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1fq4luhmp6ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1j5dq2t</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Love my sparkles</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6bqtt5gbo6ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1j5dpte</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>My lesbian flag squiggly nails</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8zsnwj79o6ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1j5cf97</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>I want my nails to last ONLY 8 hours</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j5cf97/i_want_my_nails_to_last_only_8_hours/</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1j5dfmy</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>a hint of green for the Irish 🍀</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5dfmy</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1j5csgr</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>My nails 1.5 years ago vs today</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5csgr</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1j5brea</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>dual color galaxy nails</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5brea</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1j5at8q</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Has this happened to anyone else?</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5at8q</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1j5as0c</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>💚🩷 BCB Lacquers Aesop's Fables</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5as0c</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1j5akcl</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Chat, do we like these spring nails?</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5akcl</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1j5ai4h</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dh0lmzx5v5ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1j5975x</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Asked my tech for vacay (currently in Cyprus) nails. I think she prm nailed it, personally.</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wrpadho7k5ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1j5971s</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Bl00d red nail polish I found (pls ignore the mess)</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5971s</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1j5a3vu</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>From Winter to Spring</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7dd1nqoqr5ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1j59it5</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Vampire vibes</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j59it5</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1j587fn</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>How did I do?</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/evkm6zrfc5ne1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1j57oq6</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Cat eye effect 🐱 😍 😍</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4y97hsod85ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1j57851</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>I'm in love with this beautiful design</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j57851</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1j56fzb</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Is this the start of a gel allergy or trauma to my nail?</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j56fzb</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1j55v7f</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Help my decide my birthday mani!</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j55v7f</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1j55qer</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>What happened to my nails?</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j55qer/what_happened_to_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1j567iy</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>best sculpting gel for gel x?</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j567iy/best_sculpting_gel_for_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1j560na</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Do I(/when do I) need a fill?</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j560na</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1j55pa3</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Flower Garden</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j55pa3</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1j55hkv</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>The full Sanrio aquarium set💕💫🫶🏼</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mml2kgntr4ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1j556fz</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>First time trying nail “art” if you can even call it that lol</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5pc2aazip4ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1j55498</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>I paid 60 USD / 55€, what do you say? I got them since almost one week</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rc4xs8c2p4ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1j553h7</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>before i lock in and paint them, how's this nail shape?</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j553h7</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1j54qv0</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>If you don't like AI, but buy from YN, YN has used AI on their Instagram</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgvfa3vam4ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1j54s5b</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Top coat question</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j54s5b</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1j54to3</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Red and gold</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j54to3</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1j53m2h</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Thoughts on my new set?</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j53m2h</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1j513j2</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Didier Lab Canada.... did I get ripped off?</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j513j2/didier_lab_canada_did_i_get_ripped_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1j54hd8</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>chrome isn’t chrome-ing🥺</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j54hd8</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1j548zy</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Thoughts on my nail tech</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zqiqnrmki4ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1j546k3</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Garden Party: Fine China, blue porcelain, &amp; pearls</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tllujut2i4ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1j544r2</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>‘I Beleaf In You’ 🍃 from iGel Beauty</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j544r2</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1j53zro</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>I'm obsessed with my new silver cat eyes nails</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/atk7snbag4ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1j53x4c</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Sally Hansen hard as nails</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j53x4c/sally_hansen_hard_as_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1j53n8p</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Another day, another slay from Jocelyn 🫧🌼🎀</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j53n8p</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1j538yd</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>❤️Classic Red❤️</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8wdc9r03b4ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1j534te</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Do you think it looks too bad if one of the nails is far longer than the others?</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oaxii8q3a4ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1j52pxw</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>advice on improving timing when doing a nail service</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j52pxw/advice_on_improving_timing_when_doing_a_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1j52o4k</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>What can I do about gel polish lifting from nail?</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j52o4k</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1j52mys</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>New nails coming soon.. ideas?</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l6k2qxbn64ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1j50ivk</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Shorties ❤️ BIAB on real nails</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j50ivk</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1j52jd0</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Told her I want spring vibes. I think she nailed it 💅</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8cpzxxjx54ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1j52hya</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>In LOVE with my new set!</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4jro38ym54ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1j52flt</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Spring vibes 🌺</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j52flt</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1j52e92</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Finally happy with my light blue glass nails’ effect</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/haulvrjv44ne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1j52dr7</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Cute and discreet (some would say demure) nails</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/al3hfpgs44ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1j5115j</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Chrombre nails</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5115j</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1j5263f</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Picture doesn’t do it justice but I’m so happy with it</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g13exkb734ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1j51equ</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Press Ons</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/du16jfnox3ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1j51czy</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Subtle press ons</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z3sq0o98x3ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1j515eu</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>You need all the angles to truly appreciate these beautiful nails</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j515eu</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1j513kz</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>First set of chrome coffin nails 💅</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j513kz</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1j512rs</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>spring nails</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xvylran9v3ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1j510y0</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Nails I did yesterday. Rate my work ⭐️</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j510y0</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1j502jy</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Cat eye tie dye</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vuc2yqnwn3ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1j50gwu</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Which one of you did this and why do I feel personally attacked!</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4aglchqrq3ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1j50hgd</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>nail tech is the best :3</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4zz74avvq3ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1j4zvsg</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Got my nails done. Love how they turned out!</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4zvsg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1j4zslx</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Nail Tech Appreciation Post</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4zslx</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1j4z2oc</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Aqua and gold</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wzfaeskhg3ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1j4xr3i</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Looking for good pearls for nails</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uhph2j0963ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1j4yvg0</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Looking to create this subtle/blended nail art. Any tips? Credit: 小红书 ID:Haowan091 on rednote</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f2y70wvye3ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1j4pe5v</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Any toronto nail techs that do pinched sculpture?</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j4pe5v/any_toronto_nail_techs_that_do_pinched_sculpture/</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1j4sv5g</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Quickies I did this morning</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4sv5g</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1j4y9l6</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Always ending up with cute simple nails (this time with some champagne sparkles) because my back pain doesn’t allow me to go crazy with my design ✨🥂</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tvriii2ea3ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1j4yqlq</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Gel X feels too thin? :)</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4yqlq</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1j4ykf5</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>nail sets I've done recently:)</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4ykf5</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1j4yaa2</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>My vday nails were so cute !</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/azqlnixia3ne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1j4y8xo</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Pac-Man nails</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ox2wahp8a3ne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1j4y1zl</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Bluey 💙🩵</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4pti195q83ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1j4xxc4</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Brown 🥥🧋🤎🦂✨</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/c1tp4jbp73ne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1j4xq1s</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Cut, shaped, and painted these press ons that were too long!</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9csmin4563ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1j4wzph</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Vacation nails ☀️</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4wzph</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1j4wjcw</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Londontown Chai topped with Holo Taco Everything Taco</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2rifefniw2ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1j4wavu</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Trying to plan a surprise for my girlfriend</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j4wavu/trying_to_plan_a_surprise_for_my_girlfriend/</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1j4vpit</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Something soft. What do you think? 🩷</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dr0diecbp2ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1j4vd0c</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Black chrome 🖤</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4vd0c</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1j4v5m5</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>I love my nail tech!</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4oswxnl8k2ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1j4rfza</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>im in love</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4rfza</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1j4qtbb</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>What can I do to make this look better??</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n20d5tud31ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1j4oohc</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>do you have to use gel-x tips for gel x?</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j4oohc/do_you_have_to_use_gelx_tips_for_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1j5gqe4</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>What do you do with jojoba oil post soak?</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j5gqe4/what_do_you_do_with_jojoba_oil_post_soak/</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1j5fehh</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>what was i made for? (polished for days) 💕</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5fehh</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1j5fbp6</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>VOTING for the 2024 Customer Choice Indie Polish Awards</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://forms.gle/GkcSoFCtjwV5xYoW8</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1j5f4sz</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Regret about collection. Anyone feel this way before?</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j5f4sz/regret_about_collection_anyone_feel_this_way/</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1j5e6ll</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Nail damage almost fully grown out!!</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5e6ll</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1j5e62s</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>+500 collection</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nn3zeolcs6ne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1j5e10o</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Finally healing my peeling 😌</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5e10o</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1j5dy83</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>18D cat eye gel polish</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.redgifs.com/watch/peachpuffableadouri</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1j5dc15</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>best gray based shimmers/holos?</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j5dc15/best_gray_based_shimmersholos/</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1j5d9cj</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>January Mani Roundup</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5d9cj</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1j5cwr7</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Infrared 💙💚💛🧡❤</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b2gapsfog6ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1j5cprm</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>What are your Holo Taco faves?</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j5cprm/what_are_your_holo_taco_faves/</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1j5cmt0</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Tips on how to remove a peel-off base coat better?</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5cmt0</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1j5choa</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Lacquerista lost her collection in a fire...</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j5choa/lacquerista_lost_her_collection_in_a_fire/</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1j5cfmn</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>🖤 Your Mind Is A Stream Of Color 🖤</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5cfmn</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1j5c2on</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Renaissance was not over-hyped at all, not even a little</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5c2on</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1j5byme</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>ILNP My Private Rainbow (x) over ILNP Venom</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yaeaxq0m76ne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1j5arb4</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>💚🩷 BCB Lacquers Aesop's Fables</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5arb4</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1j5aglp</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Back on my Base Coat Bull Sheet</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5aglp</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1j59y23</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Dazzle Dry - Oh My!</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wbeotp7dq5ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1j59xq9</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Dazzle Dry - Week in Provence</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r22lwv7aq5ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1j595oy</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Gorgeous in bright light but kind of drab otherwise?</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mqrsy1zkj5ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1j590ga</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Please show me your favorite weird nudes! (nude nail polish shades to be clear)</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j590ga/please_show_me_your_favorite_weird_nudes_nude/</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1j58wh8</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Miffy :D</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j58wh8</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1j51wgl</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Nail polish with Yuna’s vibe?</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bk8ol9b814ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1j56rbi</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Ethereal Lorraine Dupes?</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j56rbi/ethereal_lorraine_dupes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1j57zcs</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Anybody know the nail polish for this color?</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m1lr2p2oa5ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1j58qct</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>kur perfecting nail veil #5</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mnsxtwnlg5ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1j5827z</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Good-luck nails🍀</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5827z</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1j57g7c</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>As the young folx would say, I’m gagged</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r54ap7al65ne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1j57ccj</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Does this purple suit me ?</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j57ccj</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1j56ft8</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>I love a pastel shifty metallic!</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/egprqjavy4ne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1j56bok</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Dazzle Dry Milky Way Dupe Request!</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e7mhgi1yx4ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1j56700</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Cool beans</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j56700</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1j561kb</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>This sub and painting my nails again have saved my life</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j561kb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1j55twm</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Fancy Fish</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j55twm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1j55tjx</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Fancy Fish</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j55tjx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1j55pnq</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>If you want to feel good about your mani...</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j55pnq/if_you_want_to_feel_good_about_your_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1j55m99</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Feeling blue</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j55m99</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1j55i3l</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>ARTEMIS DEATHKISS</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uaqne2fxr4ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1j55dds</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>looking for your nails but better shade!</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5pbhizcxq4ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1j54yvr</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Lumpy and bumpy but cute!</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j54yvr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1j54tu3</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>✨Fancy Fingers✨Smith and Cult</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mq9y30gxm4ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1j54tj8</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Matching the transition to spring with a thermal nail polish</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wjhkae9vm4ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1j54dge</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Guys I am distraught that Forces of Evil is sold out and I don’t have any backups, help me dupe?</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2bdhj26jj4ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1j54724</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>First Halo Taco gift from a friend!</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j54724</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1j53ys9</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Sally Hansen Hard as Nails</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j53ys9/sally_hansen_hard_as_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1j531yt</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>This thermal is SOOOOO reactive even on my shorties!</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j531yt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1j514ja</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Skincare for hands</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j514ja/skincare_for_hands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1j50y4e</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Blue coquette nails 💙🎀</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v2rsj7pau3ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1j50wt4</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>🌈Pastel Dream🌈</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j50wt4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1j50tu8</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Slava Ukraini 🇺🇦</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/46i1sd7gt3ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1j50a9x</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Any advice on improving timing when doing a nail service ?</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j50a9x/any_advice_on_improving_timing_when_doing_a_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1j4zphz</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>How do I find my perfect nude polish without wasting money on the wrong shades?</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j4zphz/how_do_i_find_my_perfect_nude_polish_without/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1j4z8s3</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Monarch Venetian Charm: not sure how I feel about it</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4z8s3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1j4z2d6</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Anyone tried water-based Gofun (Japanese) or Kapa Nui (Hawaiian)?</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j4z2d6/anyone_tried_waterbased_gofun_japanese_or_kapa/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1j4yvbm</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>I call it... Skating Rink Carpet Skittle</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4yvbm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1j4xc5g</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Sasha</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4xc5g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1j4x9wu</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Dupe for Ethereal’s Venus Crystal?</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cm6t8vsl23ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1j4x578</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>The entire China Glaze brand is  on clearance for 50% off at Sally Beauty and Ulta this week. I’m pretty afraid for their trajectory 😭</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4x578</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1j4x2q0</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Ramadan nails</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zx9tkbmr3yme1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1j4x154</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>The sparkles are growing on me!</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/frzcepxk03ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1j4wh35</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>PSA from Hella Handmade Creations</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4wh35</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1j4vj0z</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>How to get this polish to look like the swatch?</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4vj0z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1j4vaxt</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Nail dehydrator vs acetone/alcohol</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j4vaxt/nail_dehydrator_vs_acetonealcohol/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1j4v83d</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Landscape Nails</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4v83d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1j4tsl8</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>What colors are the most popular 2025 trends?</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j4tsl8/what_colors_are_the_most_popular_2025_trends/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1j5hxmh</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>; spring/summer vibes 🩷</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ydm37wt1y7ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1j5dyqj</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Love this design</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.redgifs.com/watch/peachpuffableadouri</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1j5ds6b</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>How do my press on nails look?</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p79sb9dvo6ne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1j5cvlv</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>still need to file and shape but super proud of my first custom press on order :) it's a 24pc set!</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0vq3t04eg6ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1j5bbfp</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>I share with you the nail set I made today</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jcjw2a0826ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1j5aoki</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>My favorite manicure designs so far</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5aoki</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1j57c5d</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>my nail tech ate with this set today🤩</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j57c5d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1j56gbe</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nxh6ulo0z4ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1j56brd</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Puerto Rican flag 🇵🇷</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jzwdn5d3y4ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1j530cf</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Yesterday's work</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/29mqh8nd94ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1j51fqk</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>my spring vibe</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vvk0i1wsw3ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1j4ym6w</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Half set made for a gay party</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4ym6w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1j4v12t</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Press on beginner questions</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1j4v12t/press_on_beginner_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1j4t1p3</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Recent works hihi!</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j4t1p3</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Mar  8 08:07:51 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_03_09.xlsx
+++ b/data/collected_data/2025_03_09.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1047"/>
+  <dimension ref="A1:C1253"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18232,6 +18232,3508 @@
         </is>
       </c>
     </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1j6ca7m</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Flower nails</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dtktx0688fne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1j6bzuv</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>doodles and gems</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6bzuv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1j6bhni</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Happy International Women’s Day~ Matchy with my canned drink</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0n8wx9tayene1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1j6735a</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Just some very basic flat blue nails today ~</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6735a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1j67d5k</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>update for those who were concerned and informative about my bubble/pocket lifting</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j67d5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1j695h1</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Is it rude if I ask for these to be repainted?</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q5fxmsnx7ene1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1j6b42z</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>So cute ✨</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lyxox0yotene1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1j6atbo</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Baby blue chrome 💙🐬</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6atbo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1j6aptg</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>About to get a gel manicure soon. Recommended nail shape?</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6aptg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1j6ail3</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Been stressed and started ruining my nail beds-built up with extension gel</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9y3fxrynmene1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1j6a1r2</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Will gel polish melt when washing with warm water/blowdrying hair?</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j6a1r2/will_gel_polish_melt_when_washing_with_warm/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1j69mrj</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>First time nails!</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j69mrj/first_time_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1j69kpq</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Advice? I’m a cos student. And I’m STRUGGLING with French tips in any capacity</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q6fotu8fcene1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1j69gae</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>What shape is this?</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j69gae</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1j69dxb</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Filed the side too much</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uzhvdzeeaene1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1j68v3i</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>what would best the polish colour for my skin tone?</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gufyzc5w4ene1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1j68qrj</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>spring press ons for myself 🌷</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b8avidqn3ene1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1j68p3u</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Prep</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4hyglfw73ene1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1j68oht</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Attack on Titan Handpainted Art (his nose is straight, it's the curse of a curved canvas from birds eye view) 😆</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hb4o2dj13ene1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1j685m5</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>first time w/ gel x</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j685m5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1j67sgu</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Picnic lunch with friends 🐛</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j67sgu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1j67nws</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>some fun cat eye nails I did for my client today 🤍</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yppxdrytsdne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1j67kkm</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>I feel like I'm being gaslit about Beauty Secrets nail glue</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j67kkm/i_feel_like_im_being_gaslit_about_beauty_secrets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1j67a4h</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Do you like?</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/guouh0i6pdne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1j66qda</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>I was thinking of changing the shape of my nails.</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0hrz8l4vjdne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1j66dz1</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Took my solar nails off</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j66dz1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1j662oo</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Simple and cute</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tv5j5ktqddne1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1j65mj6</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>First Time DIY Nail Art</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j65mj6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1j65maw</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>I was encouraged to have my sister do these nails for me, I loved them!</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j1wqk7zf9dne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1j660py</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>March 🍀</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mg4n5hp7ddne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1j65cnq</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Manicure day</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x5hqk5447dne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1j655hp</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Issue in Lens application when gel extension</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j655hp/issue_in_lens_application_when_gel_extension/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1j650s0</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>This cateye look has me in such a chokehold</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2h9o7z564dne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1j64yiw</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Got these done in the city recently☺️</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j64yiw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1j64mek</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>What's the best tool for dealing with cuticles?</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j64mek/whats_the_best_tool_for_dealing_with_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1j64lrl</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>The talons of the goddess Aphrodite.</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ipzcjcr90dne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1j64dqk</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Pop of color March Nails</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j64dqk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1j64ak8</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Holo cateye layered on top of pastel cateye😻</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j7dyw41rxcne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1j649k3</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Rate my nails - first timer</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j649k3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1j647c8</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>I like short nails, but love gel… is it better to do builder gels and fills or just regular gel manicure?</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j647c8/i_like_short_nails_but_love_gel_is_it_better_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1j641d3</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Recs on commercial manicure tables?</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j641d3/recs_on_commercial_manicure_tables/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1j63oh2</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>My newest set :) What do you think?</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pto84q6hscne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1j63htr</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Why does a matte topcoat cost more?</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j63htr/why_does_a_matte_topcoat_cost_more/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1j62mnl</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Aventurine Nails!</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/imv6q9otjcne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1j62vet</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>strawberry season 🍓</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j62vet</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1j62r1x</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Something cute for spring</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u241xp5tkcne1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1j62lx3</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>My birthday nails 💅🏽💚🩵💜</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/awuwt3wnjcne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1j5z5fh</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Nail tech cut into my finger beneath my cuticle - things to watch out for while it heals?</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/18qzthkwsbne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1j60t71</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Are these good dip nails?</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j60t71</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1j60y3z</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Does the adhesive on fake nails ruin the natural nails?</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j60y3z/does_the_adhesive_on_fake_nails_ruin_the_natural/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1j60z7q</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Acrylics after losing a nail</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j60z7q/acrylics_after_losing_a_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1j61xvq</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>spring nails!!</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4sfvep88ecne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1j61oop</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Showing love to press-ons</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j61oop</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1j60wgr</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>New nails. They are simple but I wanted to show them 🥰♥️</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j60wgr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1j60jsf</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>🐈 nails</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j60jsf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1j60nox</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>1st time doing acrylics!</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j60nox</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1j60gpj</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Not very spring-like but I love it</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qxowpvao3cne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1j60cgr</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Wedding nails trial run</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l1voy6s92cne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1j6068d</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Birthday nails!</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f5e00xka0cne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1j5ztys</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>jade marble nails 💚🌟</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ye5ea8l6xbne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1j5zs83</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Can’t stop taking pictures of my nails</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5zs83</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1j5zjme</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>thoughts on my new nails?</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c1qpngudvbne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1j5zds2</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>In some angles, it's a rainbow🌈</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5zds2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1j5za6f</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Longest nails I’ve ever had</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/21fnwfnqtbne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1j5z10m</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Where to find brushes for acrylics which are vegan?</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j5z10m/where_to_find_brushes_for_acrylics_which_are_vegan/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1j5yoet</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Good reasonably priced places to get my nails done close to Portland OR?</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j5yoet/good_reasonably_priced_places_to_get_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1j5ylju</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Do my nails look off?</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vlh60i1gpbne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1j5yhpy</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Clear tips</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5yhpy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1j5y2ld</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Got new nails today!</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/id17l0r3mbne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1j5xcts</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Short and sweet</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/a4n6jsunhbne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1j5wwi2</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Builder vs Japanese gel</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j5wwi2/builder_vs_japanese_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1j5wszp</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Treated myself with some shattered glass nails this month!</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5wszp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1j5wdgb</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Allergic only to nail glue?</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j5wdgb/allergic_only_to_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1j5what</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>I'm getting my qualification end of this month but been practicing since December and trying to get content before I start taking bookings (thanks mum). Do these look "legit" ? I'm stressing about everything and getting pictures that look professional</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5what</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1j5w34l</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>how to prevent gel polish from going on skin?</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j5w34l/how_to_prevent_gel_polish_from_going_on_skin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1j5q2ac</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Vertical line in nail</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/es77cj4u7ane1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1j5uzfa</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>What do I do?</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lxbajx0e2bne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1j5vyua</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>My first human client since starting Nikki Nailed it... What do you think?</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5vyua</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1j5vy7o</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Que les parece mí práctica??</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2r5xqclm8bne1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1j5v21m</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Lucky charms nails</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rmu1yh4u2bne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1j5v15w</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>March nails 🤩💅</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5v15w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1j5i5ud</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>how do i fix a yellowish nude acrylic powder?</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j5i5ud/how_do_i_fix_a_yellowish_nude_acrylic_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1j5tlqm</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Does this look bad?</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5tlqm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1j5urtz</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>spring has sprung 🌷 what I got vs what I asked for! @daisybarbznails on ig</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5urtz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1j5unh9</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>𖤐 JADE SIREN: one of my favorite sets so far.</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2vlmdljc0bne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1j5ug22</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Lavender💜</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o4zvy7h3zane1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1j5twpm</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Press on Nails sellers</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j5twpm/press_on_nails_sellers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1j5szl3</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>How did I do?</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5szl3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1j5sock</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>What color is best in nails for dark skin?</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5o4t1s5aoane1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1j5id6f</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Hoping this is the right place to post this. I’m wondering if it’s safe to have this nail done, will explain below</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5id6f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1j5rhsa</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Our 16 yo started doing nails in July of last year. I think she has what it takes to do this as a job. Especially once she gets professional training.</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5rhsa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1j5sct4</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>MelodySusie LED/UV lamp!?</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qainpliamane1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1j5rwkk</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Got my nails done yesterday</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/00wzy58gjane1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1j5r207</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>first EVER nails</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5r207</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1j5pqih</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Rate this set 1-10</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3lxog49r5ane1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1j5p3rh</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Black Spots in Middle Nail?</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ihakkqmk1ane1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1j5owbd</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>my go to colour ❤️</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rrxh4nb40ane1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1j5ola6</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Cheapest press ons</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j5ola6/cheapest_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1j5nzon</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>I support my other half all the time but…</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/55ovw2qvt9ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1j5nw1w</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>first time getting nails done at a salon!!!</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t6f4zuk6t9ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1j6bzcr</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>I finally got itttt💜❤️</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6bzcr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1j6apwx</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Which nail colors do you get the most compliments on?</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j6apwx/which_nail_colors_do_you_get_the_most_compliments/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1j6angs</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Do Clionadh Psilocybin and Psilo-sibs look good in low lighting?</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j6angs/do_clionadh_psilocybin_and_psilosibs_look_good_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1j6ajf0</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>I seriously need this finish in every color</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6ajf0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1j6a91n</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Jelly Sandi</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jv2c7lknjene1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1j69nkv</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>First time encountering MMA acrylics - HELP!?!</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j69nkv/first_time_encountering_mma_acrylics_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1j69jh4</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Hoping these postpartum nails last!</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e9d8uvv1cene1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1j68us8</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Dupe for Mooncat Molten Lava?</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j68us8/dupe_for_mooncat_molten_lava/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1j68okq</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>One of my new fav combos!</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j68okq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1j68f7b</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Joined the broken nail club again</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j68f7b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1j676op</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>just realizing this bar lamp is also perfect for nail pics</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j676op</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1j66i62</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Pale as my soul, cold as the snow ❄️🖤</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j66i62</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1j66913</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Super shifty</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mv13zdvdfdne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1j65xyy</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Friday night reverse french mani?</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j65xyy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1j659wd</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>So Sparkly! Take Two</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6k7zmvhf6dne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1j654mc</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>As requested, my diy homemade polish, Early Girl</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/40sf9vm35dne1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1j64fm4</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Thermals like Per Se</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j64fm4/thermals_like_per_se/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1j645yu</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>NEW Spring Shades 3/7/25 @ 4PM PST</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j645yu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1j63oxn</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>I LOVE Monarch Lacquer's Rose Petal Bath! Please recommend me more Creme Shimmers!!</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j63oxn/i_love_monarch_lacquers_rose_petal_bath_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1j638d2</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Who else hates white on their nails?😁</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8bvh8plpocne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1j633gd</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Playing with Stickers!</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j633gd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1j62z9e</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>🍇 Yum yum grape jelly for Friday! 🍇</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n75edc5mmcne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1j62lmk</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>First tome giving myself a “French tip”. RIP HT Featured Guest</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j62lmk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1j62ihz</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Purgatory by BKL (Immortal Dark Mystery Bag)</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j62ihz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1j62fcq</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>My first time velvetizing a flakie magnetic and I love how different it looks at different angles! 🤯</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j62fcq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1j62cmu</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>gel top coat instead of BIAB</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j62cmu/gel_top_coat_instead_of_biab/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1j6266b</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Can you tell I have a type?</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6266b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1j62473</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>My favorite color Pixel Dust</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/edp48o2nfcne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1j621sr</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Testing if gel is fully cured? Help!</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j621sr/testing_if_gel_is_fully_cured_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1j61lvq</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>My favorite skittle I've ever done 🥹💚🩵</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j61lvq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1j60ai3</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>What’s better than one purple?? TWO PURPLES</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j60ai3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1j5zi3g</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>OPI My Address is Hollywood</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5zi3g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1j5zgtq</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Final Masquerade</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5zgtq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1j5yrih</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Baby’s first skittle</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cscc7y5gqbne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1j5yq9u</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Had to get my green on and love what I did!</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5yq9u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1j5yq0z</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>This is why I can’t have nice things.</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5yq0z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1j5yisz</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Because I’m obsessed with “glass nails”</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tdxsxz9yobne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1j5y84m</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Just got these to sort my polish!! How do I sort? By color or brand?</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q0lytr4ymbne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1j5y127</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Polish is Forever</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j5y127/polish_is_forever/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1j5xz0r</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Little bit disappointed with Clionadh?</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j5xz0r/little_bit_disappointed_with_clionadh/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1j5xuc6</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Accidentally matched my drink</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hv1twfvnkbne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1j5xaj2</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>When you fall asleep before doing your QDTC...</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ssckbr9hbne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1j5x08i</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Cashmere Chagrin</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u5v0fu9dfbne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1j5wqcd</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Graduation nails</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5wqcd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1j5wq0i</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Looking for a dupe</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hozxeoktdbne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1j5wjps</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Birthstone March Options and Comparisons</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k8uo9xyrcbne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1j5wdnc</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Can’t get enough of your love bay-beee 💛🩷💚🩵💙💜</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v8pvcg3pbbne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1j5waf9</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Questions about Mooncat polish</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j5waf9/questions_about_mooncat_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1j5w0k8</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Freehand Patterns</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5w0k8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1j5vdfa</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Just when I thought I couldn’t possibly say “NOWWW!! THIS! This ONE is for SURE my all time favorite!!!” 🤭  (please excuse the rough cuticles-nurse hands here) BUT (dare I say it) THIS ONE! THIS  MAY BE MY ALL TIME FAVE!!</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5vdfa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1j5v92p</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>ORLY Nebula is so pretty!</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/as51tsp14bne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1j5uqz5</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Base Coat For Gel Polish Frustration</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j5uqz5/base_coat_for_gel_polish_frustration/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1j5ukh6</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Confetti topper with star shaped flakes?</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j5ukh6/confetti_topper_with_star_shaped_flakes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1j5ugn0</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Nail polish names that signal feminine rage/power?</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j5ugn0/nail_polish_names_that_signal_feminine_ragepower/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1j5u98f</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>It’s finally green season</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ixiickyxxane1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1j5tnvh</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Looking for a dupe for China Glaze - Harvest Moon</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1yuyhvybuane1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1j5tepu</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>ILNP Bluebell on shorties</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w142rlhssane1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1j5taeu</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Question about red polish</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j5taeu/question_about_red_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1j5t2wh</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Floral pastel skittle for spring? “Groundbreaking” lol</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5t2wh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1j5t1cq</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>very demonic 👹 very mindful 🌷</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5t1cq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1j5sj4p</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Ready for pool weather</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5sj4p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1j5s689</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>My Nosferatu collection haul from Bees Knees Lacquer</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fz2g6855lane1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1j5s4mh</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Polish Pick Up Error?</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i3tjhxuvkane1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1j5s1ds</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Does Evil Come From Within Us by Bees Knees Lacquer on natura nails🩸🖤</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5s1ds</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1j5rti7</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>🪩I am a Disco Ball🪩</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5rti7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1j5rctt</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Experience with magnetics from Colores de Carol or Jen &amp; Berries?</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j5rctt/experience_with_magnetics_from_colores_de_carol/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1j5rbmp</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>🌸You Tart!🌸</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mhbxwtksfane1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1j5r5x9</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Obsessed with this shift</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jnnrjasvcane1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1j5q9d5</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Help for pigment stains pls</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yuznhw619ane1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1j5phew</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Can’t work today, too busy staring at my nails 🩵</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zk1hsfl34ane1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1j5oczs</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>What I asked for VS what I got</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5oczs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1j5nudf</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>The hunt continues</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j7d68beus9ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1j5nts3</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>ILNP Poison (velvetized) - kind of underwhelmed</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n71sckcps9ne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1j5nqhr</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Delighted by the Essence Magnetic</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5nqhr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1j5nlk7</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Lucky Charms</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g8vi5f52r9ne1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1j5n60e</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>House of Hades</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4xq7qj0wn9ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1j5mlv5</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Unicorn Bday Nails :)</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3hwpudeqj9ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1j5mjh0</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>A rant and a success story from a beginner</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j5mjh0/a_rant_and_a_success_story_from_a_beginner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1j5ll3r</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Minty confetti 🌿🎉</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5ll3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1j5k71y</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>I cannot access the ILNP website</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j5k71y/i_cannot_access_the_ilnp_website/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1j6axvm</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Today's design..</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d154g68lrene1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1j6amf6</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>some sets</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6amf6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1j68nyw</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Attack on Titan Handpainted Art (his nose is there, it's the curse of a curved canvas from birds eye view) 😆💕</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bveqoesv2ene1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1j689er</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Uñas bonitas que te parecen.?</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j689er</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1j63ovg</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>❤️🖕❤️ vibes tonight</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3lms0grlscne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1j63b5a</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Matte Flowers</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j63b5a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1j634u0</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Amalfi coast vibes! 💙🍑☀️</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vw17ujnwncne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1j62n4m</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>My birthday nails done by @nails_emmywynn 💅🏽💚🩵💜</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gu2cbqbxjcne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1j62gqv</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>I was in awe!!! 2 weeks in and everything is still intact</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j62gqv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1j61cbd</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Nail art with non gel polish</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1j61cbd/nail_art_with_non_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1j60ogg</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Musical themed</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j60ogg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1j5oc8a</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Love spring vibes 🤪</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5oc8a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1j5ot1m</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Recent sets</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5ot1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1j5ytai</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>My favorite job</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uvhworcrqbne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1j5yjem</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>help with client order</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5yjem</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1j5yj6g</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Clear tips</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5yj6g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1j5yhp4</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>So happy with how this hello kitty set came out 😸</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h9u2u9zqobne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1j5wxag</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Mi trabajo ☺️</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5wxag</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1j5vm4h</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Idk tried something different</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lth4vtmi6bne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1j5utqq</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>How to do prevent my nail polish from getting bubbles like this?</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5utqq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1j5unyl</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>𖤐 JADE SIREN: one of my favorite sets so far.</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2t9izmgf0bne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1j5tiar</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Hippie/Alien custom set request 👽🛸</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5tiar</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1j5lemv</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>I did my mom’s nails 😁</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/exdzbzhq69ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1j5khax</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Nightmare before Christmas nails 🎄</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5khax</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1j5j3zo</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Tried something new.</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u5x14ndsd8ne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1j5io0r</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Sesame Street Set !</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j5io0r</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Mar  9 08:08:48 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_03_09.xlsx
+++ b/data/collected_data/2025_03_09.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1253"/>
+  <dimension ref="A1:C1443"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21734,6 +21734,3236 @@
         </is>
       </c>
     </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1j71mn8</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Love my galaxy nails</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q3p6qy8izlne1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1j72rwq</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Red and blue from the 2024 archive. Have a nice day, ladies ❤️</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j72rwq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1j7259h</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Recent</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j7259h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1j719jp</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Best back drop for my new set</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vrq5n195vlne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1j6qemv</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>After Grad Week Nails 🎓</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6tp652io1jne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1j6q508</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>stained glass nails</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://youtube.com/shorts/JgpvCCM9dKE?si=Lx2BVfGfdESM0ARD</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1j6qbrq</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Question for NIL TECHS</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j6qbrq/question_for_nil_techs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1j6qvgv</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Toenail just fell off due to trauma.  Can I get a fake nail on skin??</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j6qvgv/toenail_just_fell_off_due_to_trauma_can_i_get_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1j6ro30</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Keith Haring Inspired 🎨</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6ro30</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1j70djc</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>What kind of fake nails damages your real nails the least?</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j70djc/what_kind_of_fake_nails_damages_your_real_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1j70g7f</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Gel x</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j70g7f/gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1j70bc2</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Be nice, it’s my first attempt</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j70bc2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1j6rayg</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Just finished doing these on my friend</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/89z782b29jne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1j6utii</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Arrrgh!!</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j6utii/arrrgh/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1j6sfo9</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>I get how it happens now!!</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j6sfo9/i_get_how_it_happens_now/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1j6soxl</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Press on nails over gel?</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6soxl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1j6ujpr</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>advice on missing nail kinda</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iuwim1r20kne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1j6upox</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Best product to help remove reusable press ons?</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j6upox/best_product_to_help_remove_reusable_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1j6wc4k</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>What do i do with the extra falseys that aren’t my size?</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6wc4k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1j6wpdo</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Ridge Filler or Builder Gel for dip in nail? Glue help.</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/whwhdx8vjkne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1j6x4vf</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Did press on for the first time but I need tips?</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l1dnzux1okne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1j6zcpo</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>J-hope inspo nails</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6zcpo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1j6zj3x</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>My nail personality 💅💕💘💘💘</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6zj3x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1j6znrf</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>I’m so mad help pls</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j6znrf/im_so_mad_help_pls/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1j6znmh</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>If you don’t know about Love is in the Bare by OPI then here you go!!! My favorite so far</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/33pha33cdlne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1j6zn83</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>nails suggestion</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j6zn83/nails_suggestion/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1j6z4bq</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Ready for spring - clean girl nails?</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6z4bq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1j6z06l</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Builder gel neutral glittery mani</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/20lqa7sk6lne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1j6ys3v</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Moonstone ✨</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o0qjir3b4lne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1j6yktc</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>How did my nail tech do?</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6t3oymu92lne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1j6yalp</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>(☞ﾟヮﾟ)☞</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y60gp3tczkne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1j6y179</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Birthday nails 💚💅🏻💙</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y4f44cmrwkne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1j6xzfi</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>Other tools than nail clipper?</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j6xzfi/other_tools_than_nail_clipper/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1j6xthj</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>I did full cover tips for the first time ☺️</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6xthj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1j6xsep</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>gel overlay on natural nails (:</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6xsep</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1j6xklw</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>New set!!🩷</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iphnrc79skne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1j6xg9z</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>My new set it's a work of art. I'm obsessed</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oavxvuj3rkne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1j6x8u9</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>my nail girl eats down every time</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/enjzfbd4pkne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1j6x35v</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>ISO tips and tricks using builder gel in a bottle.</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j6x35v/iso_tips_and_tricks_using_builder_gel_in_a_bottle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1j6x0ly</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>A little spring lemon squeeze</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y2gx2lixmkne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1j6wzwu</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Toothpicks to the rescue! What nail art tools do you recommend?</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6wzwu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1j6wyu7</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>I love that they glow</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/admxnuogmkne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1j6wt59</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Why do nail styles (mostly) skip over winter</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zectv7mxkkne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1j6wsuh</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>I’m in love with matte finish.</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jwimijdukkne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1j6wsgj</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Valentino not shipping to Canada ?!</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j6wsgj/valentino_not_shipping_to_canada/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1j6wq7h</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Aura nail art coming off when applying top coat</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j6wq7h/aura_nail_art_coming_off_when_applying_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1j6wft6</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Thick, ragged cuticles: oils are not making much difference. To cut or not to cut?</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j6wft6/thick_ragged_cuticles_oils_are_not_making_much/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1j6w5w2</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>New  Nails💅🏻</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6w5w2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1j6vwtf</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Help?</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6vwtf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1j6vi7b</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>St. Patty’s + Spring Vibes 👀</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/clpx8n6q8kne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1j6vgwq</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>First time with only natural nails</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/500md6qe8kne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1j6vcgy</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>My nails of the week</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6vcgy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1j6va21</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>First time using Glamnetic nails!</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b9hqb0zn6kne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1j6v9xs</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>DVOK White Night Collection + Black Base</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6v9xs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1j6v7w0</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Nun aesthetic nails</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6v7w0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1j6v3oy</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Simple but effective!</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hn2cqu915kne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1j6uy2e</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Amazing green Zoya polishes</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6uy2e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1j6uqgd</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>First time doing something out of the box, but I love them.</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q7cqfmso1kne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1j6ulnl</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Does anyone else get easily distracted by chrome nails?  I feel like I’m constantly mesmerized.</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hpcsfyzj0kne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1j6ucld</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Ready for Spring!</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6ucld</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1j6twl0</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>My first set of press-ons</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ihat6wpkujne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1j6tdmz</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Back to basics ✨</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tdcj9fj6qjne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1j6tbag</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Finally have some to post! Spring nails ❤️</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6tbag</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1j6t91b</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Easy to remove nails</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j6t91b/easy_to_remove_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1j6t1vm</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Green with envy</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eo5k30cenjne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1j6stve</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Tips?</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6stve</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1j6sa75</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>I love them! 💕</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6sa75</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1j6s01e</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Birthday nails</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mk6lr22qejne1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1j6rynd</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Critique my nails</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6rynd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1j6rwcm</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Crystal clear glitter bomb!</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/45huqatvdjne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1j6rgxe</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Plss geek over how perfect these turned out with me😍</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6rgxe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1j6rcke</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Birthday nails (little bit early lol)</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6rcke</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1j6rci9</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Just finished doing these on a friend</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t6lft8ze9jne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1j6rbmt</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>Jello jello one kill under press ons?</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j6rbmt/jello_jello_one_kill_under_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1j6rbf1</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>Jello jello one kill under press ons?</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j6rbf1/jello_jello_one_kill_under_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1j6r8gt</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>I like my new style of short nails, along with the golden hour. I think I did a good job, don’t you think? 😍🧡</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6r8gt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1j6r3b7</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Kitten stickers on colourful nails</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6r3b7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1j6qgcm</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Just a guy that loves nail fashion and doing my own nails! I normally stay subtle with my colors. But, I how this color changes with light!</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6qgcm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1j6qeuo</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>I posted a week ago because I started working at a salon. Here’s a gel set I did today</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sfis759q1jne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1j6qenf</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>New set nails</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/weda7ieo1jne1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1j6qddq</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Is there a purpose to putting rocks in this cuticle oil?</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6qddq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1j6qd91</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jzrgs0dc1jne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1j6q8la</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>My nail tech moved too far away and the new place I tried got me bleeding. I’m considering doing it from home now</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/41qzqmb90jne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1j6q6rf</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>Need help finding this cat eye shade!</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6q6rf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1j6q1rp</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Professional short mani?</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vqize3kqyine1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1j6pimb</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Subtly spring nails</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/irnt8tdeuine1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1j6pf9i</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>A little different</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mrtmi80ntine1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1j6n2lf</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Hard vs soft vs Gel X</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ngdtby91bine1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1j6m645</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>Don't wear regular polish under your gel top coat!</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6m645</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1j6m5kg</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>Base coat/ ridge filler</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j6m5kg/base_coat_ridge_filler/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1j6pe9a</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>New Style for me: Matte with Cat-Eye French Tip</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jssorv5etine1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1j6kzyk</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>I got my nails done on Monday and 4 days later the polish just fell off. What would cause this?</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6kzyk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1j6kyqz</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Nail tips that come in ONE size for practise nails?</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gkbm8gt7uhne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1j6o38w</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Just did my first indepth pedi!</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s4m8f7x1jine1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1j6p7xv</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>How to grow out press-ons cleanly?</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1j6p7xv/how_to_grow_out_pressons_cleanly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1j6owqc</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>Lil bitty shroomies 🍄</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y648ovjjpine1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1j6oud8</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>This lacquer is a perfect pink chrome!</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6oud8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1j6orrj</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>I call this the “glowy jelly beans manicure”</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zz6u0p0goine1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1j6ordb</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>Feeling lucky ☘️</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tat71bcdoine1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1j6oh8c</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>are these healthy?</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p93bxmu2mine1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1j72p0r</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>holo toppers!! tell me ur faves</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9v12uj3pcmne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1j72nr2</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>seche vite gel effect top coat ALWAYS CHIPS!!!!! WHY!</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j72nr2/seche_vite_gel_effect_top_coat_always_chips_why/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1j726z3</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>Best nail polish thinner available in Australia?</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j726z3/best_nail_polish_thinner_available_in_australia/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1j70xrk</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>I’ve had this polish for 3 years now, and it’s my first time wearing it</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5y3v4m5hrlne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1j70jru</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Bump brown gelx</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j70jru</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1j6z8xb</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>Opal decals using regular polish</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kboxb5719lne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1j6z1f9</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Mooncat - Dragon Scales</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4jow744y6lne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1j6yw34</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>Swatch sticks</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j6yw34/swatch_sticks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1j6x79p</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>Round shorties 💖🦋</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6x79p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1j6x62t</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Thorium</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j6x62t/thorium/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1j6wl2h</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Clionadh Wormhole question.</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j6wl2h/clionadh_wormhole_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1j6w2ab</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>Tip under nail bed stinging</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j6w2ab/tip_under_nail_bed_stinging/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1j6vl41</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>I’m hypnotized🔮✨</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kszphv0e9kne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1j6vi72</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Helmer Storage?</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j6vi72/helmer_storage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1j6vf01</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>I have a type - LynBDesigns haul</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mopy0gbx7kne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1j6v2vt</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Blues.</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6qm0n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1j6rtcw</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>Regular polish/laquer dupe to Gellen #101?</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6rtcw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1j6uf3h</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>Fav green polishes from Zoya</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6uf3h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1j6tyuj</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>Starrily “Oceanic Moonlight”</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wifdn7a2vjne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1j6tktx</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>Twinkled T - no labels?</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8zhmmxltrjne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1j6tfyh</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>Encounter the Blooms- Lava Barite</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/v63yjh0qqjne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1j6svum</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>What does "wait until completely dry" actually mean?</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j6svum/what_does_wait_until_completely_dry_actually_mean/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1j6skfj</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>I get it now.</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6skfj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1j6rw6x</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>This is the best find of my life!</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j6rw6x/this_is_the_best_find_of_my_life/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1j6rf1c</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>[swatch request or review request] Cracked Polish - Hidden Lagoon (from Feb Hella Handmade)</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j6rf1c/swatch_request_or_review_request_cracked_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1j6r9ve</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>Looking for this color 💕</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6r9ve</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1j6r2m6</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>Black Jelly Polish</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j6r2m6/black_jelly_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1j6qj5g</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>Polar Lights</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6qj5g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1j6k3az</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>Favorite red jellies?</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j6k3az/favorite_red_jellies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1j6qh3o</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>accidental wicked mani lol</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kq07baj92jne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1j6qf2b</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>Lemon Sucker by Holo Taco</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h02qgndr1jne1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1j6qbkz</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>Need tips on dip powder nails</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7hx0guty0jne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1j6qayz</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>Tried my hand at some freehand line art, I’m not upset with the results!</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fgderrvt0jne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1j6q52g</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>Need help finding this cat eye shade!</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6q52g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1j6q0zj</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>🍫💅</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bts8od7kyine1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1j6ptux</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>Obsessed with this color ✨</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hbzicxuxwine1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1j6p12o</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>Replace your top coat!</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6p12o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1j6omg6</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>Colorful 30lb magnet 🧲</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/at5dq2t9nine1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1j6ogl5</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>Blue Lotus (Again)</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6ogl5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1j6o5p5</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>Spring break means glitter and no nudes!</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6o5p5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1j6nrwk</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>Pictures don't do these justice. They are just too shiny</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6nrwk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1j6nht0</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>holy shift 😮</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2y3h67o9eine1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1j6nds4</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>ILNP Sugar Cube + Peach Ring</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6nds4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1j6n7h7</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>Cream formula in this shade of blue?</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6kmyg9o3cine1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1j6n48n</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>You’re Gonna Be Popular</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6n48n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1j6n0yo</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>Enjoying jelly polish so far! (Cirque)</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6n0yo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1j6mn1h</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>Happy International Women’s Day!</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6mn1h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1j6mkfd</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>To The Max</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j6mkfd/to_the_max/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1j6mbto</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>Expectation vs. Reality: Cirque Colors Gumdrop</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6mbto</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1j6m5c0</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>Her name is Rio...🎼🎸</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6m5c0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1j6m1zm</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>One more ILNP Flower Child pic before I inevitably break these babies building a new trellis in my garden today. Happy Saturday!</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tex7xzby2ine1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1j6lo3o</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>my nails look like glowy edible jelly beans</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5f66l26vzhne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1j6la5x</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>Can anyone else relate?</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/grdoezjswhne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1j6ksiq</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>Frozen Lake ❄️</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6ksiq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1j6koh3</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>I rarely see this shape on here, does anyone actually have it? I am in love with it and want to grow out my nails to look like this</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ji1lq47wrhne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1j6jxna</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>Time to reorganize and reswatch my polishes (again...)</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kmehq2nglhne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1j6jvbs</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>Something different!</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6jvbs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1j6jc8m</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>ILNP - Playlist 🍀⚡️🍋‍🟩</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6jc8m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1j6jc7y</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>do you ever just…</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qtb2n4goghne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1j6ifzi</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>My first ever non drugstore polish</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6ifzi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1j6ib1n</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>Chrome Skittle</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6ib1n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1j6i4n7</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>Thank you all so much! (+ new Spring shades)</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6i4n7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1j6hs07</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>My First Holo Taco 😍</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0m1jbqgo2hne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1j6hb3u</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>What’s your favorite green polish?</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1j6hb3u/whats_your_favorite_green_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1j6gwoa</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>It gets prettier every time I look at it🧚✨</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6gwoa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1j6ghty</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t>Clown nails</t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6ghty</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1j6g1qo</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>Bloodstone inspired nail art</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5w894mm0lgne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1j66uov</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>Extremely disappointed with Holo Taco</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uawl4hp0ldne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>1j6fefx</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>Delightful Duochromes Found at Dollar Tree</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6fefx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>1j6y24u</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>Ren Faire nails</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6y24u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>1j6y0nj</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>A very loving set</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8x00dmqmwkne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr">
+        <is>
+          <t>1j6xwkd</t>
+        </is>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>My first time</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6xwkd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="inlineStr">
+        <is>
+          <t>1j6uu89</t>
+        </is>
+      </c>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t>New nails!</t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6uu89</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="inlineStr">
+        <is>
+          <t>1j6u86f</t>
+        </is>
+      </c>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t>International Women's Day Nail Art</t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6u86f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="inlineStr">
+        <is>
+          <t>1j6si59</t>
+        </is>
+      </c>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t>March Nails</t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6si59</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="inlineStr">
+        <is>
+          <t>1j6r2r0</t>
+        </is>
+      </c>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t>my friend made me clown themed nails!!!</t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6r2r0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="inlineStr">
+        <is>
+          <t>1j6qmbx</t>
+        </is>
+      </c>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>After Grad Week Nails 🎓</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ciys5gh3jne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="inlineStr">
+        <is>
+          <t>1j6q79t</t>
+        </is>
+      </c>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>Need help finding this cat eye shade!</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6q79t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="inlineStr">
+        <is>
+          <t>1j6p7dc</t>
+        </is>
+      </c>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t>french tip brush recs?</t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1j6p7dc/french_tip_brush_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="inlineStr">
+        <is>
+          <t>1j6ougg</t>
+        </is>
+      </c>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t>Other uses for dip powder?</t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1j6ougg/other_uses_for_dip_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" t="inlineStr">
+        <is>
+          <t>1j6no0l</t>
+        </is>
+      </c>
+      <c r="B1434" t="inlineStr">
+        <is>
+          <t>Barbie Earring Magic</t>
+        </is>
+      </c>
+      <c r="C1434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6no0l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" t="inlineStr">
+        <is>
+          <t>1j6ma61</t>
+        </is>
+      </c>
+      <c r="B1435" t="inlineStr">
+        <is>
+          <t>Strawberry Shortcake</t>
+        </is>
+      </c>
+      <c r="C1435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6ma61</t>
+        </is>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" t="inlineStr">
+        <is>
+          <t>1j6lwxj</t>
+        </is>
+      </c>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t>Sondaggio smalto classico</t>
+        </is>
+      </c>
+      <c r="C1436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1j6lwxj/sondaggio_smalto_classico/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" t="inlineStr">
+        <is>
+          <t>1j6lsmq</t>
+        </is>
+      </c>
+      <c r="B1437" t="inlineStr">
+        <is>
+          <t>Hygiene</t>
+        </is>
+      </c>
+      <c r="C1437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1j6lsmq/hygiene/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" t="inlineStr">
+        <is>
+          <t>1j6kcpr</t>
+        </is>
+      </c>
+      <c r="B1438" t="inlineStr">
+        <is>
+          <t>Formula 1 inspired ✨🏎️ on XXShort tips💜</t>
+        </is>
+      </c>
+      <c r="C1438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mxn9115aphne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" t="inlineStr">
+        <is>
+          <t>1j6ioz9</t>
+        </is>
+      </c>
+      <c r="B1439" t="inlineStr">
+        <is>
+          <t>My birthday nails on myself 🩷</t>
+        </is>
+      </c>
+      <c r="C1439" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zajnraz0bhne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" t="inlineStr">
+        <is>
+          <t>1j6h55x</t>
+        </is>
+      </c>
+      <c r="B1440" t="inlineStr">
+        <is>
+          <t>My first ever attempt at painting my own nails - could be a lot neater but really pleased with how the art turned out</t>
+        </is>
+      </c>
+      <c r="C1440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6h55x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1441">
+      <c r="A1441" t="inlineStr">
+        <is>
+          <t>1j6gy6f</t>
+        </is>
+      </c>
+      <c r="B1441" t="inlineStr">
+        <is>
+          <t>What other colour than white would work here?</t>
+        </is>
+      </c>
+      <c r="C1441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vu0le8qougne1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" t="inlineStr">
+        <is>
+          <t>1j6ggw5</t>
+        </is>
+      </c>
+      <c r="B1442" t="inlineStr">
+        <is>
+          <t>Clown nails</t>
+        </is>
+      </c>
+      <c r="C1442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6ggw5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1443">
+      <c r="A1443" t="inlineStr">
+        <is>
+          <t>1j6dree</t>
+        </is>
+      </c>
+      <c r="B1443" t="inlineStr">
+        <is>
+          <t>Bright ombré</t>
+        </is>
+      </c>
+      <c r="C1443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1j6dree</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>